<commit_message>
attendnce displayed on student dashboard
</commit_message>
<xml_diff>
--- a/workbooks/SE.xlsx
+++ b/workbooks/SE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="EMIII" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,14 @@
     <sheet name="DSLAB" sheetId="8" r:id="rId8"/>
     <sheet name="CGLAB" sheetId="9" r:id="rId9"/>
     <sheet name="DLCOALAB" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet8" sheetId="11" r:id="rId11"/>
+    <sheet name="Attendance" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5331" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5333" uniqueCount="223">
   <si>
     <t xml:space="preserve">Class/Sem : </t>
   </si>
@@ -693,6 +693,12 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Total Present</t>
+  </si>
+  <si>
+    <t>Total Absent</t>
+  </si>
 </sst>
 </file>
 
@@ -881,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -957,6 +963,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1667,57 +1677,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="28"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="30"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
@@ -7704,7 +7714,7 @@
   <dimension ref="A1:AI85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7713,57 +7723,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="28"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="30"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>191</v>
       </c>
@@ -8141,7 +8151,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
@@ -11732,8 +11742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11743,6 +11753,7 @@
     <col min="6" max="6" width="9.33203125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="14" max="14" width="12.44140625" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -11845,7 +11856,7 @@
         <f>COUNTIF(DLCOALAB!E4:BP4, "P")/(COUNTIF(DLCOALAB!E4:BP4,"P")+COUNTIF(DLCOALAB!E4:BP4,"A"))*100</f>
         <v>0</v>
       </c>
-      <c r="O2" s="20">
+      <c r="O2" s="28">
         <f t="shared" ref="O2:O33" si="0">SUM(E2:N2)/10</f>
         <v>8.9230769230769234</v>
       </c>
@@ -11903,7 +11914,7 @@
         <f>COUNTIF(DLCOALAB!E5:BP5, "P")/(COUNTIF(DLCOALAB!E5:BP5,"P")+COUNTIF(DLCOALAB!E5:BP5,"A"))*100</f>
         <v>0</v>
       </c>
-      <c r="O3" s="20">
+      <c r="O3" s="28">
         <f t="shared" si="0"/>
         <v>18.923076923076923</v>
       </c>
@@ -11961,7 +11972,7 @@
         <f>COUNTIF(DLCOALAB!E6:BP6, "P")/(COUNTIF(DLCOALAB!E6:BP6,"P")+COUNTIF(DLCOALAB!E6:BP6,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O4" s="20">
+      <c r="O4" s="28">
         <f t="shared" si="0"/>
         <v>91.128205128205124</v>
       </c>
@@ -12019,7 +12030,7 @@
         <f>COUNTIF(DLCOALAB!E7:BP7, "P")/(COUNTIF(DLCOALAB!E7:BP7,"P")+COUNTIF(DLCOALAB!E7:BP7,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O5" s="20">
+      <c r="O5" s="28">
         <f t="shared" si="0"/>
         <v>93.128205128205124</v>
       </c>
@@ -12077,7 +12088,7 @@
         <f>COUNTIF(DLCOALAB!E8:BP8, "P")/(COUNTIF(DLCOALAB!E8:BP8,"P")+COUNTIF(DLCOALAB!E8:BP8,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O6" s="20">
+      <c r="O6" s="28">
         <f t="shared" si="0"/>
         <v>80.589743589743591</v>
       </c>
@@ -12135,7 +12146,7 @@
         <f>COUNTIF(DLCOALAB!E9:BP9, "P")/(COUNTIF(DLCOALAB!E9:BP9,"P")+COUNTIF(DLCOALAB!E9:BP9,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O7" s="20">
+      <c r="O7" s="28">
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
@@ -12191,11 +12202,11 @@
       </c>
       <c r="N8" s="20">
         <f>COUNTIF(DLCOALAB!E10:BP10, "P")/(COUNTIF(DLCOALAB!E10:BP10,"P")+COUNTIF(DLCOALAB!E10:BP10,"A"))*100</f>
-        <v>100</v>
-      </c>
-      <c r="O8" s="20">
+        <v>0</v>
+      </c>
+      <c r="O8" s="28">
         <f t="shared" si="0"/>
-        <v>94.461538461538467</v>
+        <v>84.461538461538467</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -12251,7 +12262,7 @@
         <f>COUNTIF(DLCOALAB!E11:BP11, "P")/(COUNTIF(DLCOALAB!E11:BP11,"P")+COUNTIF(DLCOALAB!E11:BP11,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O9" s="20">
+      <c r="O9" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -12309,7 +12320,7 @@
         <f>COUNTIF(DLCOALAB!E12:BP12, "P")/(COUNTIF(DLCOALAB!E12:BP12,"P")+COUNTIF(DLCOALAB!E12:BP12,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O10" s="20">
+      <c r="O10" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -12367,7 +12378,7 @@
         <f>COUNTIF(DLCOALAB!E13:BP13, "P")/(COUNTIF(DLCOALAB!E13:BP13,"P")+COUNTIF(DLCOALAB!E13:BP13,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O11" s="20">
+      <c r="O11" s="28">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
@@ -12425,7 +12436,7 @@
         <f>COUNTIF(DLCOALAB!E14:BP14, "P")/(COUNTIF(DLCOALAB!E14:BP14,"P")+COUNTIF(DLCOALAB!E14:BP14,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O12" s="20">
+      <c r="O12" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -12483,7 +12494,7 @@
         <f>COUNTIF(DLCOALAB!E15:BP15, "P")/(COUNTIF(DLCOALAB!E15:BP15,"P")+COUNTIF(DLCOALAB!E15:BP15,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O13" s="20">
+      <c r="O13" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -12541,7 +12552,7 @@
         <f>COUNTIF(DLCOALAB!E16:BP16, "P")/(COUNTIF(DLCOALAB!E16:BP16,"P")+COUNTIF(DLCOALAB!E16:BP16,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O14" s="20">
+      <c r="O14" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -12599,7 +12610,7 @@
         <f>COUNTIF(DLCOALAB!E17:BP17, "P")/(COUNTIF(DLCOALAB!E17:BP17,"P")+COUNTIF(DLCOALAB!E17:BP17,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O15" s="20">
+      <c r="O15" s="28">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
@@ -12657,7 +12668,7 @@
         <f>COUNTIF(DLCOALAB!E18:BP18, "P")/(COUNTIF(DLCOALAB!E18:BP18,"P")+COUNTIF(DLCOALAB!E18:BP18,"A"))*100</f>
         <v>0</v>
       </c>
-      <c r="O16" s="20">
+      <c r="O16" s="28">
         <f t="shared" si="0"/>
         <v>31.333333333333332</v>
       </c>
@@ -12715,7 +12726,7 @@
         <f>COUNTIF(DLCOALAB!E19:BP19, "P")/(COUNTIF(DLCOALAB!E19:BP19,"P")+COUNTIF(DLCOALAB!E19:BP19,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O17" s="20">
+      <c r="O17" s="28">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
@@ -12773,7 +12784,7 @@
         <f>COUNTIF(DLCOALAB!E20:BP20, "P")/(COUNTIF(DLCOALAB!E20:BP20,"P")+COUNTIF(DLCOALAB!E20:BP20,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O18" s="20">
+      <c r="O18" s="28">
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
@@ -12831,7 +12842,7 @@
         <f>COUNTIF(DLCOALAB!E21:BP21, "P")/(COUNTIF(DLCOALAB!E21:BP21,"P")+COUNTIF(DLCOALAB!E21:BP21,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O19" s="20">
+      <c r="O19" s="28">
         <f t="shared" si="0"/>
         <v>99.230769230769241</v>
       </c>
@@ -12889,7 +12900,7 @@
         <f>COUNTIF(DLCOALAB!E22:BP22, "P")/(COUNTIF(DLCOALAB!E22:BP22,"P")+COUNTIF(DLCOALAB!E22:BP22,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O20" s="20">
+      <c r="O20" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -12947,7 +12958,7 @@
         <f>COUNTIF(DLCOALAB!E23:BP23, "P")/(COUNTIF(DLCOALAB!E23:BP23,"P")+COUNTIF(DLCOALAB!E23:BP23,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O21" s="20">
+      <c r="O21" s="28">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
@@ -13005,7 +13016,7 @@
         <f>COUNTIF(DLCOALAB!E24:BP24, "P")/(COUNTIF(DLCOALAB!E24:BP24,"P")+COUNTIF(DLCOALAB!E24:BP24,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O22" s="20">
+      <c r="O22" s="28">
         <f t="shared" si="0"/>
         <v>99.230769230769241</v>
       </c>
@@ -13063,7 +13074,7 @@
         <f>COUNTIF(DLCOALAB!E25:BP25, "P")/(COUNTIF(DLCOALAB!E25:BP25,"P")+COUNTIF(DLCOALAB!E25:BP25,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O23" s="20">
+      <c r="O23" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -13121,7 +13132,7 @@
         <f>COUNTIF(DLCOALAB!E26:BP26, "P")/(COUNTIF(DLCOALAB!E26:BP26,"P")+COUNTIF(DLCOALAB!E26:BP26,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O24" s="20">
+      <c r="O24" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -13179,7 +13190,7 @@
         <f>COUNTIF(DLCOALAB!E27:BP27, "P")/(COUNTIF(DLCOALAB!E27:BP27,"P")+COUNTIF(DLCOALAB!E27:BP27,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O25" s="20">
+      <c r="O25" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -13237,7 +13248,7 @@
         <f>COUNTIF(DLCOALAB!E28:BP28, "P")/(COUNTIF(DLCOALAB!E28:BP28,"P")+COUNTIF(DLCOALAB!E28:BP28,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O26" s="20">
+      <c r="O26" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -13295,7 +13306,7 @@
         <f>COUNTIF(DLCOALAB!E29:BP29, "P")/(COUNTIF(DLCOALAB!E29:BP29,"P")+COUNTIF(DLCOALAB!E29:BP29,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O27" s="20">
+      <c r="O27" s="28">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
@@ -13353,7 +13364,7 @@
         <f>COUNTIF(DLCOALAB!E30:BP30, "P")/(COUNTIF(DLCOALAB!E30:BP30,"P")+COUNTIF(DLCOALAB!E30:BP30,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O28" s="20">
+      <c r="O28" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -13411,7 +13422,7 @@
         <f>COUNTIF(DLCOALAB!E31:BP31, "P")/(COUNTIF(DLCOALAB!E31:BP31,"P")+COUNTIF(DLCOALAB!E31:BP31,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O29" s="20">
+      <c r="O29" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -13469,7 +13480,7 @@
         <f>COUNTIF(DLCOALAB!E32:BP32, "P")/(COUNTIF(DLCOALAB!E32:BP32,"P")+COUNTIF(DLCOALAB!E32:BP32,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O30" s="20">
+      <c r="O30" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -13527,7 +13538,7 @@
         <f>COUNTIF(DLCOALAB!E33:BP33, "P")/(COUNTIF(DLCOALAB!E33:BP33,"P")+COUNTIF(DLCOALAB!E33:BP33,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O31" s="20">
+      <c r="O31" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -13585,7 +13596,7 @@
         <f>COUNTIF(DLCOALAB!E34:BP34, "P")/(COUNTIF(DLCOALAB!E34:BP34,"P")+COUNTIF(DLCOALAB!E34:BP34,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O32" s="20">
+      <c r="O32" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -13643,7 +13654,7 @@
         <f>COUNTIF(DLCOALAB!E35:BP35, "P")/(COUNTIF(DLCOALAB!E35:BP35,"P")+COUNTIF(DLCOALAB!E35:BP35,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O33" s="20">
+      <c r="O33" s="28">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -13701,7 +13712,7 @@
         <f>COUNTIF(DLCOALAB!E36:BP36, "P")/(COUNTIF(DLCOALAB!E36:BP36,"P")+COUNTIF(DLCOALAB!E36:BP36,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O34" s="20">
+      <c r="O34" s="28">
         <f t="shared" ref="O34:O65" si="1">SUM(E34:N34)/10</f>
         <v>100</v>
       </c>
@@ -13759,7 +13770,7 @@
         <f>COUNTIF(DLCOALAB!E37:BP37, "P")/(COUNTIF(DLCOALAB!E37:BP37,"P")+COUNTIF(DLCOALAB!E37:BP37,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O35" s="20">
+      <c r="O35" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -13817,7 +13828,7 @@
         <f>COUNTIF(DLCOALAB!E38:BP38, "P")/(COUNTIF(DLCOALAB!E38:BP38,"P")+COUNTIF(DLCOALAB!E38:BP38,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O36" s="20">
+      <c r="O36" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -13875,7 +13886,7 @@
         <f>COUNTIF(DLCOALAB!E39:BP39, "P")/(COUNTIF(DLCOALAB!E39:BP39,"P")+COUNTIF(DLCOALAB!E39:BP39,"A"))*100</f>
         <v>0</v>
       </c>
-      <c r="O37" s="20">
+      <c r="O37" s="28">
         <f t="shared" si="1"/>
         <v>31.333333333333332</v>
       </c>
@@ -13933,7 +13944,7 @@
         <f>COUNTIF(DLCOALAB!E40:BP40, "P")/(COUNTIF(DLCOALAB!E40:BP40,"P")+COUNTIF(DLCOALAB!E40:BP40,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O38" s="20">
+      <c r="O38" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -13991,7 +14002,7 @@
         <f>COUNTIF(DLCOALAB!E41:BP41, "P")/(COUNTIF(DLCOALAB!E41:BP41,"P")+COUNTIF(DLCOALAB!E41:BP41,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O39" s="20">
+      <c r="O39" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14049,7 +14060,7 @@
         <f>COUNTIF(DLCOALAB!E42:BP42, "P")/(COUNTIF(DLCOALAB!E42:BP42,"P")+COUNTIF(DLCOALAB!E42:BP42,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O40" s="20">
+      <c r="O40" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14107,7 +14118,7 @@
         <f>COUNTIF(DLCOALAB!E43:BP43, "P")/(COUNTIF(DLCOALAB!E43:BP43,"P")+COUNTIF(DLCOALAB!E43:BP43,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O41" s="20">
+      <c r="O41" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14165,7 +14176,7 @@
         <f>COUNTIF(DLCOALAB!E44:BP44, "P")/(COUNTIF(DLCOALAB!E44:BP44,"P")+COUNTIF(DLCOALAB!E44:BP44,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O42" s="20">
+      <c r="O42" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14223,7 +14234,7 @@
         <f>COUNTIF(DLCOALAB!E45:BP45, "P")/(COUNTIF(DLCOALAB!E45:BP45,"P")+COUNTIF(DLCOALAB!E45:BP45,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O43" s="20">
+      <c r="O43" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14281,7 +14292,7 @@
         <f>COUNTIF(DLCOALAB!E46:BP46, "P")/(COUNTIF(DLCOALAB!E46:BP46,"P")+COUNTIF(DLCOALAB!E46:BP46,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O44" s="20">
+      <c r="O44" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14339,7 +14350,7 @@
         <f>COUNTIF(DLCOALAB!E47:BP47, "P")/(COUNTIF(DLCOALAB!E47:BP47,"P")+COUNTIF(DLCOALAB!E47:BP47,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O45" s="20">
+      <c r="O45" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14397,7 +14408,7 @@
         <f>COUNTIF(DLCOALAB!E48:BP48, "P")/(COUNTIF(DLCOALAB!E48:BP48,"P")+COUNTIF(DLCOALAB!E48:BP48,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O46" s="20">
+      <c r="O46" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14455,7 +14466,7 @@
         <f>COUNTIF(DLCOALAB!E49:BP49, "P")/(COUNTIF(DLCOALAB!E49:BP49,"P")+COUNTIF(DLCOALAB!E49:BP49,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O47" s="20">
+      <c r="O47" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14513,7 +14524,7 @@
         <f>COUNTIF(DLCOALAB!E50:BP50, "P")/(COUNTIF(DLCOALAB!E50:BP50,"P")+COUNTIF(DLCOALAB!E50:BP50,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O48" s="20">
+      <c r="O48" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14571,7 +14582,7 @@
         <f>COUNTIF(DLCOALAB!E51:BP51, "P")/(COUNTIF(DLCOALAB!E51:BP51,"P")+COUNTIF(DLCOALAB!E51:BP51,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O49" s="20">
+      <c r="O49" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14629,7 +14640,7 @@
         <f>COUNTIF(DLCOALAB!E52:BP52, "P")/(COUNTIF(DLCOALAB!E52:BP52,"P")+COUNTIF(DLCOALAB!E52:BP52,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O50" s="20">
+      <c r="O50" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14687,7 +14698,7 @@
         <f>COUNTIF(DLCOALAB!E53:BP53, "P")/(COUNTIF(DLCOALAB!E53:BP53,"P")+COUNTIF(DLCOALAB!E53:BP53,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O51" s="20">
+      <c r="O51" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14745,7 +14756,7 @@
         <f>COUNTIF(DLCOALAB!E54:BP54, "P")/(COUNTIF(DLCOALAB!E54:BP54,"P")+COUNTIF(DLCOALAB!E54:BP54,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O52" s="20">
+      <c r="O52" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14803,7 +14814,7 @@
         <f>COUNTIF(DLCOALAB!E55:BP55, "P")/(COUNTIF(DLCOALAB!E55:BP55,"P")+COUNTIF(DLCOALAB!E55:BP55,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O53" s="20">
+      <c r="O53" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14861,7 +14872,7 @@
         <f>COUNTIF(DLCOALAB!E56:BP56, "P")/(COUNTIF(DLCOALAB!E56:BP56,"P")+COUNTIF(DLCOALAB!E56:BP56,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O54" s="20">
+      <c r="O54" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14919,7 +14930,7 @@
         <f>COUNTIF(DLCOALAB!E57:BP57, "P")/(COUNTIF(DLCOALAB!E57:BP57,"P")+COUNTIF(DLCOALAB!E57:BP57,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O55" s="20">
+      <c r="O55" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -14977,7 +14988,7 @@
         <f>COUNTIF(DLCOALAB!E58:BP58, "P")/(COUNTIF(DLCOALAB!E58:BP58,"P")+COUNTIF(DLCOALAB!E58:BP58,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O56" s="20">
+      <c r="O56" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -15035,7 +15046,7 @@
         <f>COUNTIF(DLCOALAB!E59:BP59, "P")/(COUNTIF(DLCOALAB!E59:BP59,"P")+COUNTIF(DLCOALAB!E59:BP59,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O57" s="20">
+      <c r="O57" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -15093,7 +15104,7 @@
         <f>COUNTIF(DLCOALAB!E60:BP60, "P")/(COUNTIF(DLCOALAB!E60:BP60,"P")+COUNTIF(DLCOALAB!E60:BP60,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O58" s="20">
+      <c r="O58" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -15151,7 +15162,7 @@
         <f>COUNTIF(DLCOALAB!E61:BP61, "P")/(COUNTIF(DLCOALAB!E61:BP61,"P")+COUNTIF(DLCOALAB!E61:BP61,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O59" s="20">
+      <c r="O59" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -15209,7 +15220,7 @@
         <f>COUNTIF(DLCOALAB!E62:BP62, "P")/(COUNTIF(DLCOALAB!E62:BP62,"P")+COUNTIF(DLCOALAB!E62:BP62,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O60" s="20">
+      <c r="O60" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -15267,7 +15278,7 @@
         <f>COUNTIF(DLCOALAB!E63:BP63, "P")/(COUNTIF(DLCOALAB!E63:BP63,"P")+COUNTIF(DLCOALAB!E63:BP63,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O61" s="20">
+      <c r="O61" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -15325,7 +15336,7 @@
         <f>COUNTIF(DLCOALAB!E64:BP64, "P")/(COUNTIF(DLCOALAB!E64:BP64,"P")+COUNTIF(DLCOALAB!E64:BP64,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O62" s="20">
+      <c r="O62" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -15383,7 +15394,7 @@
         <f>COUNTIF(DLCOALAB!E65:BP65, "P")/(COUNTIF(DLCOALAB!E65:BP65,"P")+COUNTIF(DLCOALAB!E65:BP65,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O63" s="20">
+      <c r="O63" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -15441,7 +15452,7 @@
         <f>COUNTIF(DLCOALAB!E66:BP66, "P")/(COUNTIF(DLCOALAB!E66:BP66,"P")+COUNTIF(DLCOALAB!E66:BP66,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O64" s="20">
+      <c r="O64" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -15499,7 +15510,7 @@
         <f>COUNTIF(DLCOALAB!E67:BP67, "P")/(COUNTIF(DLCOALAB!E67:BP67,"P")+COUNTIF(DLCOALAB!E67:BP67,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O65" s="20">
+      <c r="O65" s="28">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -15557,8 +15568,8 @@
         <f>COUNTIF(DLCOALAB!E68:BP68, "P")/(COUNTIF(DLCOALAB!E68:BP68,"P")+COUNTIF(DLCOALAB!E68:BP68,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O66" s="20">
-        <f t="shared" ref="O66:O97" si="2">SUM(E66:N66)/10</f>
+      <c r="O66" s="28">
+        <f t="shared" ref="O66:O83" si="2">SUM(E66:N66)/10</f>
         <v>100</v>
       </c>
     </row>
@@ -15615,7 +15626,7 @@
         <f>COUNTIF(DLCOALAB!E69:BP69, "P")/(COUNTIF(DLCOALAB!E69:BP69,"P")+COUNTIF(DLCOALAB!E69:BP69,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O67" s="20">
+      <c r="O67" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -15673,7 +15684,7 @@
         <f>COUNTIF(DLCOALAB!E70:BP70, "P")/(COUNTIF(DLCOALAB!E70:BP70,"P")+COUNTIF(DLCOALAB!E70:BP70,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O68" s="20">
+      <c r="O68" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -15731,7 +15742,7 @@
         <f>COUNTIF(DLCOALAB!E71:BP71, "P")/(COUNTIF(DLCOALAB!E71:BP71,"P")+COUNTIF(DLCOALAB!E71:BP71,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O69" s="20">
+      <c r="O69" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -15789,7 +15800,7 @@
         <f>COUNTIF(DLCOALAB!E72:BP72, "P")/(COUNTIF(DLCOALAB!E72:BP72,"P")+COUNTIF(DLCOALAB!E72:BP72,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O70" s="20">
+      <c r="O70" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -15847,7 +15858,7 @@
         <f>COUNTIF(DLCOALAB!E73:BP73, "P")/(COUNTIF(DLCOALAB!E73:BP73,"P")+COUNTIF(DLCOALAB!E73:BP73,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O71" s="20">
+      <c r="O71" s="28">
         <f t="shared" si="2"/>
         <v>96.666666666666657</v>
       </c>
@@ -15905,7 +15916,7 @@
         <f>COUNTIF(DLCOALAB!E74:BP74, "P")/(COUNTIF(DLCOALAB!E74:BP74,"P")+COUNTIF(DLCOALAB!E74:BP74,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O72" s="20">
+      <c r="O72" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -15963,7 +15974,7 @@
         <f>COUNTIF(DLCOALAB!E75:BP75, "P")/(COUNTIF(DLCOALAB!E75:BP75,"P")+COUNTIF(DLCOALAB!E75:BP75,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O73" s="20">
+      <c r="O73" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -16021,7 +16032,7 @@
         <f>COUNTIF(DLCOALAB!E76:BP76, "P")/(COUNTIF(DLCOALAB!E76:BP76,"P")+COUNTIF(DLCOALAB!E76:BP76,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O74" s="20">
+      <c r="O74" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -16079,7 +16090,7 @@
         <f>COUNTIF(DLCOALAB!E77:BP77, "P")/(COUNTIF(DLCOALAB!E77:BP77,"P")+COUNTIF(DLCOALAB!E77:BP77,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O75" s="20">
+      <c r="O75" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -16137,7 +16148,7 @@
         <f>COUNTIF(DLCOALAB!E78:BP78, "P")/(COUNTIF(DLCOALAB!E78:BP78,"P")+COUNTIF(DLCOALAB!E78:BP78,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O76" s="20">
+      <c r="O76" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -16195,7 +16206,7 @@
         <f>COUNTIF(DLCOALAB!E79:BP79, "P")/(COUNTIF(DLCOALAB!E79:BP79,"P")+COUNTIF(DLCOALAB!E79:BP79,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O77" s="20">
+      <c r="O77" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -16253,7 +16264,7 @@
         <f>COUNTIF(DLCOALAB!E80:BP80, "P")/(COUNTIF(DLCOALAB!E80:BP80,"P")+COUNTIF(DLCOALAB!E80:BP80,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O78" s="20">
+      <c r="O78" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -16311,7 +16322,7 @@
         <f>COUNTIF(DLCOALAB!E81:BP81, "P")/(COUNTIF(DLCOALAB!E81:BP81,"P")+COUNTIF(DLCOALAB!E81:BP81,"A"))*100</f>
         <v>0</v>
       </c>
-      <c r="O79" s="20">
+      <c r="O79" s="28">
         <f t="shared" si="2"/>
         <v>34.666666666666664</v>
       </c>
@@ -16369,7 +16380,7 @@
         <f>COUNTIF(DLCOALAB!E82:BP82, "P")/(COUNTIF(DLCOALAB!E82:BP82,"P")+COUNTIF(DLCOALAB!E82:BP82,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O80" s="20">
+      <c r="O80" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -16427,7 +16438,7 @@
         <f>COUNTIF(DLCOALAB!E83:BP83, "P")/(COUNTIF(DLCOALAB!E83:BP83,"P")+COUNTIF(DLCOALAB!E83:BP83,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O81" s="20">
+      <c r="O81" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -16485,7 +16496,7 @@
         <f>COUNTIF(DLCOALAB!E84:BP84, "P")/(COUNTIF(DLCOALAB!E84:BP84,"P")+COUNTIF(DLCOALAB!E84:BP84,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O82" s="20">
+      <c r="O82" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -16543,7 +16554,7 @@
         <f>COUNTIF(DLCOALAB!E85:BP85, "P")/(COUNTIF(DLCOALAB!E85:BP85,"P")+COUNTIF(DLCOALAB!E85:BP85,"A"))*100</f>
         <v>100</v>
       </c>
-      <c r="O83" s="20">
+      <c r="O83" s="28">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -16573,57 +16584,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="28"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="30"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
@@ -20770,57 +20781,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="28"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="30"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>191</v>
       </c>
@@ -25135,57 +25146,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="28"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="30"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>191</v>
       </c>
@@ -29152,10 +29163,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI85"/>
+  <dimension ref="A1:BF87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AY89" sqref="AY89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29164,57 +29175,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="28"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="30"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>191</v>
       </c>
@@ -33547,7 +33558,7 @@
       <c r="AH80" s="20"/>
       <c r="AI80" s="20"/>
     </row>
-    <row r="81" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:58" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="6">
         <v>78</v>
       </c>
@@ -33602,7 +33613,7 @@
       <c r="AH81" s="20"/>
       <c r="AI81" s="20"/>
     </row>
-    <row r="82" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:58" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="6">
         <v>79</v>
       </c>
@@ -33657,7 +33668,7 @@
       <c r="AH82" s="20"/>
       <c r="AI82" s="20"/>
     </row>
-    <row r="83" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:58" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="6">
         <v>80</v>
       </c>
@@ -33712,7 +33723,7 @@
       <c r="AH83" s="20"/>
       <c r="AI83" s="20"/>
     </row>
-    <row r="84" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:58" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="8">
         <v>81</v>
       </c>
@@ -33767,7 +33778,7 @@
       <c r="AH84" s="20"/>
       <c r="AI84" s="20"/>
     </row>
-    <row r="85" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:58" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="8">
         <v>82</v>
       </c>
@@ -33821,6 +33832,448 @@
       <c r="AG85" s="20"/>
       <c r="AH85" s="20"/>
       <c r="AI85" s="20"/>
+    </row>
+    <row r="86" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A86" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="E86">
+        <f>COUNTIF(E4:E85,"P")</f>
+        <v>77</v>
+      </c>
+      <c r="F86">
+        <f t="shared" ref="F86:BF86" si="0">COUNTIF(F4:F85,"P")</f>
+        <v>77</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AF86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AG86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AJ86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AM86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AO86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AP86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AQ86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AR86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AS86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AU86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AV86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AW86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AX86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AY86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AZ86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="BA86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="BB86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="BC86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="BD86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="BE86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="BF86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A87" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E87">
+        <f>COUNTIF(E4:E85,"A")</f>
+        <v>5</v>
+      </c>
+      <c r="F87">
+        <f t="shared" ref="F87:BF87" si="1">COUNTIF(F4:F85,"A")</f>
+        <v>5</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AH87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AI87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AJ87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AK87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AL87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AO87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AP87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AQ87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AR87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AS87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AT87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AV87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AW87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AX87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AY87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AZ87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="BA87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="BB87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="BC87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="BD87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="BE87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="BF87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -33862,57 +34315,57 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="28"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="30"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>191</v>
       </c>
@@ -37888,57 +38341,57 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="28"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="30"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>191</v>
       </c>
@@ -42085,57 +42538,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="28"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="30"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>191</v>
       </c>
@@ -46111,57 +46564,57 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="29" t="s">
         <v>208</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="28"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="30"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>191</v>
       </c>

</xml_diff>

<commit_message>
styled SE dashboard, and also added a progress circle
</commit_message>
<xml_diff>
--- a/workbooks/SE.xlsx
+++ b/workbooks/SE.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5751" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5919" uniqueCount="222">
   <si>
     <t xml:space="preserve">Class/Sem : </t>
   </si>
@@ -643,6 +643,12 @@
     <t>Name of Course : OOPM</t>
   </si>
   <si>
+    <t>22/09</t>
+  </si>
+  <si>
+    <t>23/09</t>
+  </si>
+  <si>
     <t>Name of Course : DS LAB</t>
   </si>
   <si>
@@ -966,27 +972,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="41">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -8705,18 +8691,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8746,7 +8732,7 @@
       <c r="C1" s="31"/>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -12735,18 +12721,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12786,37 +12772,37 @@
         <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -12850,7 +12836,7 @@
       </c>
       <c r="I2" s="20">
         <f>COUNTIF(OOPM!E4:BP4, "P")/(COUNTIF(OOPM!E4:BP4,"P")+COUNTIF(OOPM!E4:BP4,"A"))*100</f>
-        <v>25</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="J2" s="20">
         <f>COUNTIF(DSGT!E4:BP4, "P")/(COUNTIF(DSGT!E4:BP4,"P")+COUNTIF(DSGT!E4:BP4,"A"))*100</f>
@@ -12874,7 +12860,7 @@
       </c>
       <c r="O2" s="27">
         <f t="shared" ref="O2:O33" si="0">SUM(E2:N2)/10</f>
-        <v>8.8157894736842106</v>
+        <v>7.9824561403508767</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -12908,7 +12894,7 @@
       </c>
       <c r="I3" s="20">
         <f>COUNTIF(OOPM!E5:BP5, "P")/(COUNTIF(OOPM!E5:BP5,"P")+COUNTIF(OOPM!E5:BP5,"A"))*100</f>
-        <v>25</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="J3" s="20">
         <f>COUNTIF(DSGT!E5:BP5, "P")/(COUNTIF(DSGT!E5:BP5,"P")+COUNTIF(DSGT!E5:BP5,"A"))*100</f>
@@ -12932,7 +12918,7 @@
       </c>
       <c r="O3" s="27">
         <f t="shared" si="0"/>
-        <v>18.815789473684212</v>
+        <v>19.649122807017545</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -12966,7 +12952,7 @@
       </c>
       <c r="I4" s="20">
         <f>COUNTIF(OOPM!E6:BP6, "P")/(COUNTIF(OOPM!E6:BP6,"P")+COUNTIF(OOPM!E6:BP6,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J4" s="20">
         <f>COUNTIF(DSGT!E6:BP6, "P")/(COUNTIF(DSGT!E6:BP6,"P")+COUNTIF(DSGT!E6:BP6,"A"))*100</f>
@@ -12990,7 +12976,7 @@
       </c>
       <c r="O4" s="27">
         <f t="shared" si="0"/>
-        <v>91.535087719298247</v>
+        <v>90.701754385964904</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -13024,7 +13010,7 @@
       </c>
       <c r="I5" s="20">
         <f>COUNTIF(OOPM!E7:BP7, "P")/(COUNTIF(OOPM!E7:BP7,"P")+COUNTIF(OOPM!E7:BP7,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J5" s="20">
         <f>COUNTIF(DSGT!E7:BP7, "P")/(COUNTIF(DSGT!E7:BP7,"P")+COUNTIF(DSGT!E7:BP7,"A"))*100</f>
@@ -13048,7 +13034,7 @@
       </c>
       <c r="O5" s="27">
         <f t="shared" si="0"/>
-        <v>92.587719298245617</v>
+        <v>91.754385964912274</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -13082,7 +13068,7 @@
       </c>
       <c r="I6" s="20">
         <f>COUNTIF(OOPM!E8:BP8, "P")/(COUNTIF(OOPM!E8:BP8,"P")+COUNTIF(OOPM!E8:BP8,"A"))*100</f>
-        <v>75</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="J6" s="20">
         <f>COUNTIF(DSGT!E8:BP8, "P")/(COUNTIF(DSGT!E8:BP8,"P")+COUNTIF(DSGT!E8:BP8,"A"))*100</f>
@@ -13106,7 +13092,7 @@
       </c>
       <c r="O6" s="27">
         <f t="shared" si="0"/>
-        <v>86.535087719298247</v>
+        <v>87.368421052631589</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -13140,7 +13126,7 @@
       </c>
       <c r="I7" s="20">
         <f>COUNTIF(OOPM!E9:BP9, "P")/(COUNTIF(OOPM!E9:BP9,"P")+COUNTIF(OOPM!E9:BP9,"A"))*100</f>
-        <v>75</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="J7" s="20">
         <f>COUNTIF(DSGT!E9:BP9, "P")/(COUNTIF(DSGT!E9:BP9,"P")+COUNTIF(DSGT!E9:BP9,"A"))*100</f>
@@ -13164,7 +13150,7 @@
       </c>
       <c r="O7" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>97.280701754385959</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -13198,7 +13184,7 @@
       </c>
       <c r="I8" s="20">
         <f>COUNTIF(OOPM!E10:BP10, "P")/(COUNTIF(OOPM!E10:BP10,"P")+COUNTIF(OOPM!E10:BP10,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J8" s="20">
         <f>COUNTIF(DSGT!E10:BP10, "P")/(COUNTIF(DSGT!E10:BP10,"P")+COUNTIF(DSGT!E10:BP10,"A"))*100</f>
@@ -13222,7 +13208,7 @@
       </c>
       <c r="O8" s="27">
         <f t="shared" si="0"/>
-        <v>85.39473684210526</v>
+        <v>84.561403508771917</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -13256,7 +13242,7 @@
       </c>
       <c r="I9" s="20">
         <f>COUNTIF(OOPM!E11:BP11, "P")/(COUNTIF(OOPM!E11:BP11,"P")+COUNTIF(OOPM!E11:BP11,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J9" s="20">
         <f>COUNTIF(DSGT!E11:BP11, "P")/(COUNTIF(DSGT!E11:BP11,"P")+COUNTIF(DSGT!E11:BP11,"A"))*100</f>
@@ -13280,7 +13266,7 @@
       </c>
       <c r="O9" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -13314,7 +13300,7 @@
       </c>
       <c r="I10" s="20">
         <f>COUNTIF(OOPM!E12:BP12, "P")/(COUNTIF(OOPM!E12:BP12,"P")+COUNTIF(OOPM!E12:BP12,"A"))*100</f>
-        <v>75</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="J10" s="20">
         <f>COUNTIF(DSGT!E12:BP12, "P")/(COUNTIF(DSGT!E12:BP12,"P")+COUNTIF(DSGT!E12:BP12,"A"))*100</f>
@@ -13338,7 +13324,7 @@
       </c>
       <c r="O10" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>97.280701754385959</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -13372,7 +13358,7 @@
       </c>
       <c r="I11" s="20">
         <f>COUNTIF(OOPM!E13:BP13, "P")/(COUNTIF(OOPM!E13:BP13,"P")+COUNTIF(OOPM!E13:BP13,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J11" s="20">
         <f>COUNTIF(DSGT!E13:BP13, "P")/(COUNTIF(DSGT!E13:BP13,"P")+COUNTIF(DSGT!E13:BP13,"A"))*100</f>
@@ -13396,7 +13382,7 @@
       </c>
       <c r="O11" s="27">
         <f t="shared" si="0"/>
-        <v>90.921052631578945</v>
+        <v>90.087719298245617</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -13430,7 +13416,7 @@
       </c>
       <c r="I12" s="20">
         <f>COUNTIF(OOPM!E14:BP14, "P")/(COUNTIF(OOPM!E14:BP14,"P")+COUNTIF(OOPM!E14:BP14,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J12" s="20">
         <f>COUNTIF(DSGT!E14:BP14, "P")/(COUNTIF(DSGT!E14:BP14,"P")+COUNTIF(DSGT!E14:BP14,"A"))*100</f>
@@ -13454,7 +13440,7 @@
       </c>
       <c r="O12" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -13488,7 +13474,7 @@
       </c>
       <c r="I13" s="20">
         <f>COUNTIF(OOPM!E15:BP15, "P")/(COUNTIF(OOPM!E15:BP15,"P")+COUNTIF(OOPM!E15:BP15,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J13" s="20">
         <f>COUNTIF(DSGT!E15:BP15, "P")/(COUNTIF(DSGT!E15:BP15,"P")+COUNTIF(DSGT!E15:BP15,"A"))*100</f>
@@ -13512,7 +13498,7 @@
       </c>
       <c r="O13" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -13546,7 +13532,7 @@
       </c>
       <c r="I14" s="20">
         <f>COUNTIF(OOPM!E16:BP16, "P")/(COUNTIF(OOPM!E16:BP16,"P")+COUNTIF(OOPM!E16:BP16,"A"))*100</f>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="J14" s="20">
         <f>COUNTIF(DSGT!E16:BP16, "P")/(COUNTIF(DSGT!E16:BP16,"P")+COUNTIF(DSGT!E16:BP16,"A"))*100</f>
@@ -13570,7 +13556,7 @@
       </c>
       <c r="O14" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>93.94736842105263</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -13604,7 +13590,7 @@
       </c>
       <c r="I15" s="20">
         <f>COUNTIF(OOPM!E17:BP17, "P")/(COUNTIF(OOPM!E17:BP17,"P")+COUNTIF(OOPM!E17:BP17,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J15" s="20">
         <f>COUNTIF(DSGT!E17:BP17, "P")/(COUNTIF(DSGT!E17:BP17,"P")+COUNTIF(DSGT!E17:BP17,"A"))*100</f>
@@ -13628,7 +13614,7 @@
       </c>
       <c r="O15" s="27">
         <f t="shared" si="0"/>
-        <v>91.44736842105263</v>
+        <v>90.614035087719301</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -13662,7 +13648,7 @@
       </c>
       <c r="I16" s="20">
         <f>COUNTIF(OOPM!E18:BP18, "P")/(COUNTIF(OOPM!E18:BP18,"P")+COUNTIF(OOPM!E18:BP18,"A"))*100</f>
-        <v>25</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="J16" s="20">
         <f>COUNTIF(DSGT!E18:BP18, "P")/(COUNTIF(DSGT!E18:BP18,"P")+COUNTIF(DSGT!E18:BP18,"A"))*100</f>
@@ -13686,7 +13672,7 @@
       </c>
       <c r="O16" s="27">
         <f t="shared" si="0"/>
-        <v>24.780701754385962</v>
+        <v>23.947368421052627</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -13720,7 +13706,7 @@
       </c>
       <c r="I17" s="20">
         <f>COUNTIF(OOPM!E19:BP19, "P")/(COUNTIF(OOPM!E19:BP19,"P")+COUNTIF(OOPM!E19:BP19,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J17" s="20">
         <f>COUNTIF(DSGT!E19:BP19, "P")/(COUNTIF(DSGT!E19:BP19,"P")+COUNTIF(DSGT!E19:BP19,"A"))*100</f>
@@ -13744,7 +13730,7 @@
       </c>
       <c r="O17" s="27">
         <f t="shared" si="0"/>
-        <v>86.44736842105263</v>
+        <v>85.614035087719301</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -13778,7 +13764,7 @@
       </c>
       <c r="I18" s="20">
         <f>COUNTIF(OOPM!E20:BP20, "P")/(COUNTIF(OOPM!E20:BP20,"P")+COUNTIF(OOPM!E20:BP20,"A"))*100</f>
-        <v>75</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="J18" s="20">
         <f>COUNTIF(DSGT!E20:BP20, "P")/(COUNTIF(DSGT!E20:BP20,"P")+COUNTIF(DSGT!E20:BP20,"A"))*100</f>
@@ -13802,7 +13788,7 @@
       </c>
       <c r="O18" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>97.280701754385959</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -13836,7 +13822,7 @@
       </c>
       <c r="I19" s="20">
         <f>COUNTIF(OOPM!E21:BP21, "P")/(COUNTIF(OOPM!E21:BP21,"P")+COUNTIF(OOPM!E21:BP21,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J19" s="20">
         <f>COUNTIF(DSGT!E21:BP21, "P")/(COUNTIF(DSGT!E21:BP21,"P")+COUNTIF(DSGT!E21:BP21,"A"))*100</f>
@@ -13860,7 +13846,7 @@
       </c>
       <c r="O19" s="27">
         <f t="shared" si="0"/>
-        <v>95.921052631578945</v>
+        <v>95.087719298245617</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -13894,7 +13880,7 @@
       </c>
       <c r="I20" s="20">
         <f>COUNTIF(OOPM!E22:BP22, "P")/(COUNTIF(OOPM!E22:BP22,"P")+COUNTIF(OOPM!E22:BP22,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J20" s="20">
         <f>COUNTIF(DSGT!E22:BP22, "P")/(COUNTIF(DSGT!E22:BP22,"P")+COUNTIF(DSGT!E22:BP22,"A"))*100</f>
@@ -13918,7 +13904,7 @@
       </c>
       <c r="O20" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -13952,7 +13938,7 @@
       </c>
       <c r="I21" s="20">
         <f>COUNTIF(OOPM!E23:BP23, "P")/(COUNTIF(OOPM!E23:BP23,"P")+COUNTIF(OOPM!E23:BP23,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J21" s="20">
         <f>COUNTIF(DSGT!E23:BP23, "P")/(COUNTIF(DSGT!E23:BP23,"P")+COUNTIF(DSGT!E23:BP23,"A"))*100</f>
@@ -13976,7 +13962,7 @@
       </c>
       <c r="O21" s="27">
         <f t="shared" si="0"/>
-        <v>90.921052631578945</v>
+        <v>90.087719298245617</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -14010,7 +13996,7 @@
       </c>
       <c r="I22" s="20">
         <f>COUNTIF(OOPM!E24:BP24, "P")/(COUNTIF(OOPM!E24:BP24,"P")+COUNTIF(OOPM!E24:BP24,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J22" s="20">
         <f>COUNTIF(DSGT!E24:BP24, "P")/(COUNTIF(DSGT!E24:BP24,"P")+COUNTIF(DSGT!E24:BP24,"A"))*100</f>
@@ -14034,7 +14020,7 @@
       </c>
       <c r="O22" s="27">
         <f t="shared" si="0"/>
-        <v>95.921052631578945</v>
+        <v>95.087719298245617</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -14068,7 +14054,7 @@
       </c>
       <c r="I23" s="20">
         <f>COUNTIF(OOPM!E25:BP25, "P")/(COUNTIF(OOPM!E25:BP25,"P")+COUNTIF(OOPM!E25:BP25,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J23" s="20">
         <f>COUNTIF(DSGT!E25:BP25, "P")/(COUNTIF(DSGT!E25:BP25,"P")+COUNTIF(DSGT!E25:BP25,"A"))*100</f>
@@ -14092,7 +14078,7 @@
       </c>
       <c r="O23" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -14126,7 +14112,7 @@
       </c>
       <c r="I24" s="20">
         <f>COUNTIF(OOPM!E26:BP26, "P")/(COUNTIF(OOPM!E26:BP26,"P")+COUNTIF(OOPM!E26:BP26,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J24" s="20">
         <f>COUNTIF(DSGT!E26:BP26, "P")/(COUNTIF(DSGT!E26:BP26,"P")+COUNTIF(DSGT!E26:BP26,"A"))*100</f>
@@ -14150,7 +14136,7 @@
       </c>
       <c r="O24" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -14184,7 +14170,7 @@
       </c>
       <c r="I25" s="20">
         <f>COUNTIF(OOPM!E27:BP27, "P")/(COUNTIF(OOPM!E27:BP27,"P")+COUNTIF(OOPM!E27:BP27,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J25" s="20">
         <f>COUNTIF(DSGT!E27:BP27, "P")/(COUNTIF(DSGT!E27:BP27,"P")+COUNTIF(DSGT!E27:BP27,"A"))*100</f>
@@ -14208,7 +14194,7 @@
       </c>
       <c r="O25" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -14242,7 +14228,7 @@
       </c>
       <c r="I26" s="20">
         <f>COUNTIF(OOPM!E28:BP28, "P")/(COUNTIF(OOPM!E28:BP28,"P")+COUNTIF(OOPM!E28:BP28,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J26" s="20">
         <f>COUNTIF(DSGT!E28:BP28, "P")/(COUNTIF(DSGT!E28:BP28,"P")+COUNTIF(DSGT!E28:BP28,"A"))*100</f>
@@ -14266,7 +14252,7 @@
       </c>
       <c r="O26" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -14300,7 +14286,7 @@
       </c>
       <c r="I27" s="20">
         <f>COUNTIF(OOPM!E29:BP29, "P")/(COUNTIF(OOPM!E29:BP29,"P")+COUNTIF(OOPM!E29:BP29,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J27" s="20">
         <f>COUNTIF(DSGT!E29:BP29, "P")/(COUNTIF(DSGT!E29:BP29,"P")+COUNTIF(DSGT!E29:BP29,"A"))*100</f>
@@ -14324,7 +14310,7 @@
       </c>
       <c r="O27" s="27">
         <f t="shared" si="0"/>
-        <v>91.44736842105263</v>
+        <v>90.614035087719301</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -14358,7 +14344,7 @@
       </c>
       <c r="I28" s="20">
         <f>COUNTIF(OOPM!E30:BP30, "P")/(COUNTIF(OOPM!E30:BP30,"P")+COUNTIF(OOPM!E30:BP30,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J28" s="20">
         <f>COUNTIF(DSGT!E30:BP30, "P")/(COUNTIF(DSGT!E30:BP30,"P")+COUNTIF(DSGT!E30:BP30,"A"))*100</f>
@@ -14382,7 +14368,7 @@
       </c>
       <c r="O28" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -14416,7 +14402,7 @@
       </c>
       <c r="I29" s="20">
         <f>COUNTIF(OOPM!E31:BP31, "P")/(COUNTIF(OOPM!E31:BP31,"P")+COUNTIF(OOPM!E31:BP31,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J29" s="20">
         <f>COUNTIF(DSGT!E31:BP31, "P")/(COUNTIF(DSGT!E31:BP31,"P")+COUNTIF(DSGT!E31:BP31,"A"))*100</f>
@@ -14440,7 +14426,7 @@
       </c>
       <c r="O29" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -14474,7 +14460,7 @@
       </c>
       <c r="I30" s="20">
         <f>COUNTIF(OOPM!E32:BP32, "P")/(COUNTIF(OOPM!E32:BP32,"P")+COUNTIF(OOPM!E32:BP32,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J30" s="20">
         <f>COUNTIF(DSGT!E32:BP32, "P")/(COUNTIF(DSGT!E32:BP32,"P")+COUNTIF(DSGT!E32:BP32,"A"))*100</f>
@@ -14498,7 +14484,7 @@
       </c>
       <c r="O30" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -14532,7 +14518,7 @@
       </c>
       <c r="I31" s="20">
         <f>COUNTIF(OOPM!E33:BP33, "P")/(COUNTIF(OOPM!E33:BP33,"P")+COUNTIF(OOPM!E33:BP33,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J31" s="20">
         <f>COUNTIF(DSGT!E33:BP33, "P")/(COUNTIF(DSGT!E33:BP33,"P")+COUNTIF(DSGT!E33:BP33,"A"))*100</f>
@@ -14556,7 +14542,7 @@
       </c>
       <c r="O31" s="27">
         <f t="shared" si="0"/>
-        <v>95.921052631578945</v>
+        <v>95.087719298245617</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -14590,7 +14576,7 @@
       </c>
       <c r="I32" s="20">
         <f>COUNTIF(OOPM!E34:BP34, "P")/(COUNTIF(OOPM!E34:BP34,"P")+COUNTIF(OOPM!E34:BP34,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J32" s="20">
         <f>COUNTIF(DSGT!E34:BP34, "P")/(COUNTIF(DSGT!E34:BP34,"P")+COUNTIF(DSGT!E34:BP34,"A"))*100</f>
@@ -14614,7 +14600,7 @@
       </c>
       <c r="O32" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -14648,7 +14634,7 @@
       </c>
       <c r="I33" s="20">
         <f>COUNTIF(OOPM!E35:BP35, "P")/(COUNTIF(OOPM!E35:BP35,"P")+COUNTIF(OOPM!E35:BP35,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J33" s="20">
         <f>COUNTIF(DSGT!E35:BP35, "P")/(COUNTIF(DSGT!E35:BP35,"P")+COUNTIF(DSGT!E35:BP35,"A"))*100</f>
@@ -14672,7 +14658,7 @@
       </c>
       <c r="O33" s="27">
         <f t="shared" si="0"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -14706,7 +14692,7 @@
       </c>
       <c r="I34" s="20">
         <f>COUNTIF(OOPM!E36:BP36, "P")/(COUNTIF(OOPM!E36:BP36,"P")+COUNTIF(OOPM!E36:BP36,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J34" s="20">
         <f>COUNTIF(DSGT!E36:BP36, "P")/(COUNTIF(DSGT!E36:BP36,"P")+COUNTIF(DSGT!E36:BP36,"A"))*100</f>
@@ -14730,7 +14716,7 @@
       </c>
       <c r="O34" s="27">
         <f t="shared" ref="O34:O65" si="1">SUM(E34:N34)/10</f>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -14764,7 +14750,7 @@
       </c>
       <c r="I35" s="20">
         <f>COUNTIF(OOPM!E37:BP37, "P")/(COUNTIF(OOPM!E37:BP37,"P")+COUNTIF(OOPM!E37:BP37,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J35" s="20">
         <f>COUNTIF(DSGT!E37:BP37, "P")/(COUNTIF(DSGT!E37:BP37,"P")+COUNTIF(DSGT!E37:BP37,"A"))*100</f>
@@ -14788,7 +14774,7 @@
       </c>
       <c r="O35" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -14822,7 +14808,7 @@
       </c>
       <c r="I36" s="20">
         <f>COUNTIF(OOPM!E38:BP38, "P")/(COUNTIF(OOPM!E38:BP38,"P")+COUNTIF(OOPM!E38:BP38,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J36" s="20">
         <f>COUNTIF(DSGT!E38:BP38, "P")/(COUNTIF(DSGT!E38:BP38,"P")+COUNTIF(DSGT!E38:BP38,"A"))*100</f>
@@ -14846,7 +14832,7 @@
       </c>
       <c r="O36" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -14880,7 +14866,7 @@
       </c>
       <c r="I37" s="20">
         <f>COUNTIF(OOPM!E39:BP39, "P")/(COUNTIF(OOPM!E39:BP39,"P")+COUNTIF(OOPM!E39:BP39,"A"))*100</f>
-        <v>25</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="J37" s="20">
         <f>COUNTIF(DSGT!E39:BP39, "P")/(COUNTIF(DSGT!E39:BP39,"P")+COUNTIF(DSGT!E39:BP39,"A"))*100</f>
@@ -14904,7 +14890,7 @@
       </c>
       <c r="O37" s="27">
         <f t="shared" si="1"/>
-        <v>24.780701754385962</v>
+        <v>25.614035087719294</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -14938,7 +14924,7 @@
       </c>
       <c r="I38" s="20">
         <f>COUNTIF(OOPM!E40:BP40, "P")/(COUNTIF(OOPM!E40:BP40,"P")+COUNTIF(OOPM!E40:BP40,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J38" s="20">
         <f>COUNTIF(DSGT!E40:BP40, "P")/(COUNTIF(DSGT!E40:BP40,"P")+COUNTIF(DSGT!E40:BP40,"A"))*100</f>
@@ -14962,7 +14948,7 @@
       </c>
       <c r="O38" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
@@ -14996,7 +14982,7 @@
       </c>
       <c r="I39" s="20">
         <f>COUNTIF(OOPM!E41:BP41, "P")/(COUNTIF(OOPM!E41:BP41,"P")+COUNTIF(OOPM!E41:BP41,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J39" s="20">
         <f>COUNTIF(DSGT!E41:BP41, "P")/(COUNTIF(DSGT!E41:BP41,"P")+COUNTIF(DSGT!E41:BP41,"A"))*100</f>
@@ -15020,7 +15006,7 @@
       </c>
       <c r="O39" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -15054,7 +15040,7 @@
       </c>
       <c r="I40" s="20">
         <f>COUNTIF(OOPM!E42:BP42, "P")/(COUNTIF(OOPM!E42:BP42,"P")+COUNTIF(OOPM!E42:BP42,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J40" s="20">
         <f>COUNTIF(DSGT!E42:BP42, "P")/(COUNTIF(DSGT!E42:BP42,"P")+COUNTIF(DSGT!E42:BP42,"A"))*100</f>
@@ -15078,7 +15064,7 @@
       </c>
       <c r="O40" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -15112,7 +15098,7 @@
       </c>
       <c r="I41" s="20">
         <f>COUNTIF(OOPM!E43:BP43, "P")/(COUNTIF(OOPM!E43:BP43,"P")+COUNTIF(OOPM!E43:BP43,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J41" s="20">
         <f>COUNTIF(DSGT!E43:BP43, "P")/(COUNTIF(DSGT!E43:BP43,"P")+COUNTIF(DSGT!E43:BP43,"A"))*100</f>
@@ -15136,7 +15122,7 @@
       </c>
       <c r="O41" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
@@ -15170,7 +15156,7 @@
       </c>
       <c r="I42" s="20">
         <f>COUNTIF(OOPM!E44:BP44, "P")/(COUNTIF(OOPM!E44:BP44,"P")+COUNTIF(OOPM!E44:BP44,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J42" s="20">
         <f>COUNTIF(DSGT!E44:BP44, "P")/(COUNTIF(DSGT!E44:BP44,"P")+COUNTIF(DSGT!E44:BP44,"A"))*100</f>
@@ -15194,7 +15180,7 @@
       </c>
       <c r="O42" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -15228,7 +15214,7 @@
       </c>
       <c r="I43" s="20">
         <f>COUNTIF(OOPM!E45:BP45, "P")/(COUNTIF(OOPM!E45:BP45,"P")+COUNTIF(OOPM!E45:BP45,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J43" s="20">
         <f>COUNTIF(DSGT!E45:BP45, "P")/(COUNTIF(DSGT!E45:BP45,"P")+COUNTIF(DSGT!E45:BP45,"A"))*100</f>
@@ -15252,7 +15238,7 @@
       </c>
       <c r="O43" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
@@ -15286,7 +15272,7 @@
       </c>
       <c r="I44" s="20">
         <f>COUNTIF(OOPM!E46:BP46, "P")/(COUNTIF(OOPM!E46:BP46,"P")+COUNTIF(OOPM!E46:BP46,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J44" s="20">
         <f>COUNTIF(DSGT!E46:BP46, "P")/(COUNTIF(DSGT!E46:BP46,"P")+COUNTIF(DSGT!E46:BP46,"A"))*100</f>
@@ -15310,7 +15296,7 @@
       </c>
       <c r="O44" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -15344,7 +15330,7 @@
       </c>
       <c r="I45" s="20">
         <f>COUNTIF(OOPM!E47:BP47, "P")/(COUNTIF(OOPM!E47:BP47,"P")+COUNTIF(OOPM!E47:BP47,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J45" s="20">
         <f>COUNTIF(DSGT!E47:BP47, "P")/(COUNTIF(DSGT!E47:BP47,"P")+COUNTIF(DSGT!E47:BP47,"A"))*100</f>
@@ -15368,7 +15354,7 @@
       </c>
       <c r="O45" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
@@ -15402,7 +15388,7 @@
       </c>
       <c r="I46" s="20">
         <f>COUNTIF(OOPM!E48:BP48, "P")/(COUNTIF(OOPM!E48:BP48,"P")+COUNTIF(OOPM!E48:BP48,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J46" s="20">
         <f>COUNTIF(DSGT!E48:BP48, "P")/(COUNTIF(DSGT!E48:BP48,"P")+COUNTIF(DSGT!E48:BP48,"A"))*100</f>
@@ -15426,7 +15412,7 @@
       </c>
       <c r="O46" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -15460,7 +15446,7 @@
       </c>
       <c r="I47" s="20">
         <f>COUNTIF(OOPM!E49:BP49, "P")/(COUNTIF(OOPM!E49:BP49,"P")+COUNTIF(OOPM!E49:BP49,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J47" s="20">
         <f>COUNTIF(DSGT!E49:BP49, "P")/(COUNTIF(DSGT!E49:BP49,"P")+COUNTIF(DSGT!E49:BP49,"A"))*100</f>
@@ -15484,7 +15470,7 @@
       </c>
       <c r="O47" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
@@ -15518,7 +15504,7 @@
       </c>
       <c r="I48" s="20">
         <f>COUNTIF(OOPM!E50:BP50, "P")/(COUNTIF(OOPM!E50:BP50,"P")+COUNTIF(OOPM!E50:BP50,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J48" s="20">
         <f>COUNTIF(DSGT!E50:BP50, "P")/(COUNTIF(DSGT!E50:BP50,"P")+COUNTIF(DSGT!E50:BP50,"A"))*100</f>
@@ -15542,7 +15528,7 @@
       </c>
       <c r="O48" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
@@ -15576,7 +15562,7 @@
       </c>
       <c r="I49" s="20">
         <f>COUNTIF(OOPM!E51:BP51, "P")/(COUNTIF(OOPM!E51:BP51,"P")+COUNTIF(OOPM!E51:BP51,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J49" s="20">
         <f>COUNTIF(DSGT!E51:BP51, "P")/(COUNTIF(DSGT!E51:BP51,"P")+COUNTIF(DSGT!E51:BP51,"A"))*100</f>
@@ -15600,7 +15586,7 @@
       </c>
       <c r="O49" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
@@ -15634,7 +15620,7 @@
       </c>
       <c r="I50" s="20">
         <f>COUNTIF(OOPM!E52:BP52, "P")/(COUNTIF(OOPM!E52:BP52,"P")+COUNTIF(OOPM!E52:BP52,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J50" s="20">
         <f>COUNTIF(DSGT!E52:BP52, "P")/(COUNTIF(DSGT!E52:BP52,"P")+COUNTIF(DSGT!E52:BP52,"A"))*100</f>
@@ -15658,7 +15644,7 @@
       </c>
       <c r="O50" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -15692,7 +15678,7 @@
       </c>
       <c r="I51" s="20">
         <f>COUNTIF(OOPM!E53:BP53, "P")/(COUNTIF(OOPM!E53:BP53,"P")+COUNTIF(OOPM!E53:BP53,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J51" s="20">
         <f>COUNTIF(DSGT!E53:BP53, "P")/(COUNTIF(DSGT!E53:BP53,"P")+COUNTIF(DSGT!E53:BP53,"A"))*100</f>
@@ -15716,7 +15702,7 @@
       </c>
       <c r="O51" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
@@ -15750,7 +15736,7 @@
       </c>
       <c r="I52" s="20">
         <f>COUNTIF(OOPM!E54:BP54, "P")/(COUNTIF(OOPM!E54:BP54,"P")+COUNTIF(OOPM!E54:BP54,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J52" s="20">
         <f>COUNTIF(DSGT!E54:BP54, "P")/(COUNTIF(DSGT!E54:BP54,"P")+COUNTIF(DSGT!E54:BP54,"A"))*100</f>
@@ -15774,7 +15760,7 @@
       </c>
       <c r="O52" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -15808,7 +15794,7 @@
       </c>
       <c r="I53" s="20">
         <f>COUNTIF(OOPM!E55:BP55, "P")/(COUNTIF(OOPM!E55:BP55,"P")+COUNTIF(OOPM!E55:BP55,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J53" s="20">
         <f>COUNTIF(DSGT!E55:BP55, "P")/(COUNTIF(DSGT!E55:BP55,"P")+COUNTIF(DSGT!E55:BP55,"A"))*100</f>
@@ -15832,7 +15818,7 @@
       </c>
       <c r="O53" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
@@ -15866,7 +15852,7 @@
       </c>
       <c r="I54" s="20">
         <f>COUNTIF(OOPM!E56:BP56, "P")/(COUNTIF(OOPM!E56:BP56,"P")+COUNTIF(OOPM!E56:BP56,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J54" s="20">
         <f>COUNTIF(DSGT!E56:BP56, "P")/(COUNTIF(DSGT!E56:BP56,"P")+COUNTIF(DSGT!E56:BP56,"A"))*100</f>
@@ -15890,7 +15876,7 @@
       </c>
       <c r="O54" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -15924,7 +15910,7 @@
       </c>
       <c r="I55" s="20">
         <f>COUNTIF(OOPM!E57:BP57, "P")/(COUNTIF(OOPM!E57:BP57,"P")+COUNTIF(OOPM!E57:BP57,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J55" s="20">
         <f>COUNTIF(DSGT!E57:BP57, "P")/(COUNTIF(DSGT!E57:BP57,"P")+COUNTIF(DSGT!E57:BP57,"A"))*100</f>
@@ -15948,7 +15934,7 @@
       </c>
       <c r="O55" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
@@ -15982,7 +15968,7 @@
       </c>
       <c r="I56" s="20">
         <f>COUNTIF(OOPM!E58:BP58, "P")/(COUNTIF(OOPM!E58:BP58,"P")+COUNTIF(OOPM!E58:BP58,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J56" s="20">
         <f>COUNTIF(DSGT!E58:BP58, "P")/(COUNTIF(DSGT!E58:BP58,"P")+COUNTIF(DSGT!E58:BP58,"A"))*100</f>
@@ -16006,7 +15992,7 @@
       </c>
       <c r="O56" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
@@ -16040,7 +16026,7 @@
       </c>
       <c r="I57" s="20">
         <f>COUNTIF(OOPM!E59:BP59, "P")/(COUNTIF(OOPM!E59:BP59,"P")+COUNTIF(OOPM!E59:BP59,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J57" s="20">
         <f>COUNTIF(DSGT!E59:BP59, "P")/(COUNTIF(DSGT!E59:BP59,"P")+COUNTIF(DSGT!E59:BP59,"A"))*100</f>
@@ -16064,7 +16050,7 @@
       </c>
       <c r="O57" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
@@ -16098,7 +16084,7 @@
       </c>
       <c r="I58" s="20">
         <f>COUNTIF(OOPM!E60:BP60, "P")/(COUNTIF(OOPM!E60:BP60,"P")+COUNTIF(OOPM!E60:BP60,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J58" s="20">
         <f>COUNTIF(DSGT!E60:BP60, "P")/(COUNTIF(DSGT!E60:BP60,"P")+COUNTIF(DSGT!E60:BP60,"A"))*100</f>
@@ -16122,7 +16108,7 @@
       </c>
       <c r="O58" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
@@ -16156,7 +16142,7 @@
       </c>
       <c r="I59" s="20">
         <f>COUNTIF(OOPM!E61:BP61, "P")/(COUNTIF(OOPM!E61:BP61,"P")+COUNTIF(OOPM!E61:BP61,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J59" s="20">
         <f>COUNTIF(DSGT!E61:BP61, "P")/(COUNTIF(DSGT!E61:BP61,"P")+COUNTIF(DSGT!E61:BP61,"A"))*100</f>
@@ -16180,7 +16166,7 @@
       </c>
       <c r="O59" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
@@ -16214,7 +16200,7 @@
       </c>
       <c r="I60" s="20">
         <f>COUNTIF(OOPM!E62:BP62, "P")/(COUNTIF(OOPM!E62:BP62,"P")+COUNTIF(OOPM!E62:BP62,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J60" s="20">
         <f>COUNTIF(DSGT!E62:BP62, "P")/(COUNTIF(DSGT!E62:BP62,"P")+COUNTIF(DSGT!E62:BP62,"A"))*100</f>
@@ -16238,7 +16224,7 @@
       </c>
       <c r="O60" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
@@ -16272,7 +16258,7 @@
       </c>
       <c r="I61" s="20">
         <f>COUNTIF(OOPM!E63:BP63, "P")/(COUNTIF(OOPM!E63:BP63,"P")+COUNTIF(OOPM!E63:BP63,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J61" s="20">
         <f>COUNTIF(DSGT!E63:BP63, "P")/(COUNTIF(DSGT!E63:BP63,"P")+COUNTIF(DSGT!E63:BP63,"A"))*100</f>
@@ -16296,7 +16282,7 @@
       </c>
       <c r="O61" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
@@ -16330,7 +16316,7 @@
       </c>
       <c r="I62" s="20">
         <f>COUNTIF(OOPM!E64:BP64, "P")/(COUNTIF(OOPM!E64:BP64,"P")+COUNTIF(OOPM!E64:BP64,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J62" s="20">
         <f>COUNTIF(DSGT!E64:BP64, "P")/(COUNTIF(DSGT!E64:BP64,"P")+COUNTIF(DSGT!E64:BP64,"A"))*100</f>
@@ -16354,7 +16340,7 @@
       </c>
       <c r="O62" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
@@ -16388,7 +16374,7 @@
       </c>
       <c r="I63" s="20">
         <f>COUNTIF(OOPM!E65:BP65, "P")/(COUNTIF(OOPM!E65:BP65,"P")+COUNTIF(OOPM!E65:BP65,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J63" s="20">
         <f>COUNTIF(DSGT!E65:BP65, "P")/(COUNTIF(DSGT!E65:BP65,"P")+COUNTIF(DSGT!E65:BP65,"A"))*100</f>
@@ -16412,7 +16398,7 @@
       </c>
       <c r="O63" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
@@ -16446,7 +16432,7 @@
       </c>
       <c r="I64" s="20">
         <f>COUNTIF(OOPM!E66:BP66, "P")/(COUNTIF(OOPM!E66:BP66,"P")+COUNTIF(OOPM!E66:BP66,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J64" s="20">
         <f>COUNTIF(DSGT!E66:BP66, "P")/(COUNTIF(DSGT!E66:BP66,"P")+COUNTIF(DSGT!E66:BP66,"A"))*100</f>
@@ -16470,7 +16456,7 @@
       </c>
       <c r="O64" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
@@ -16504,7 +16490,7 @@
       </c>
       <c r="I65" s="20">
         <f>COUNTIF(OOPM!E67:BP67, "P")/(COUNTIF(OOPM!E67:BP67,"P")+COUNTIF(OOPM!E67:BP67,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J65" s="20">
         <f>COUNTIF(DSGT!E67:BP67, "P")/(COUNTIF(DSGT!E67:BP67,"P")+COUNTIF(DSGT!E67:BP67,"A"))*100</f>
@@ -16528,7 +16514,7 @@
       </c>
       <c r="O65" s="27">
         <f t="shared" si="1"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
@@ -16562,7 +16548,7 @@
       </c>
       <c r="I66" s="20">
         <f>COUNTIF(OOPM!E68:BP68, "P")/(COUNTIF(OOPM!E68:BP68,"P")+COUNTIF(OOPM!E68:BP68,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J66" s="20">
         <f>COUNTIF(DSGT!E68:BP68, "P")/(COUNTIF(DSGT!E68:BP68,"P")+COUNTIF(DSGT!E68:BP68,"A"))*100</f>
@@ -16585,8 +16571,8 @@
         <v>100</v>
       </c>
       <c r="O66" s="27">
-        <f t="shared" ref="O66:O83" si="2">SUM(E66:N66)/10</f>
-        <v>96.44736842105263</v>
+        <f t="shared" ref="O66:O97" si="2">SUM(E66:N66)/10</f>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
@@ -16620,7 +16606,7 @@
       </c>
       <c r="I67" s="20">
         <f>COUNTIF(OOPM!E69:BP69, "P")/(COUNTIF(OOPM!E69:BP69,"P")+COUNTIF(OOPM!E69:BP69,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J67" s="20">
         <f>COUNTIF(DSGT!E69:BP69, "P")/(COUNTIF(DSGT!E69:BP69,"P")+COUNTIF(DSGT!E69:BP69,"A"))*100</f>
@@ -16644,7 +16630,7 @@
       </c>
       <c r="O67" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
@@ -16678,7 +16664,7 @@
       </c>
       <c r="I68" s="20">
         <f>COUNTIF(OOPM!E70:BP70, "P")/(COUNTIF(OOPM!E70:BP70,"P")+COUNTIF(OOPM!E70:BP70,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J68" s="20">
         <f>COUNTIF(DSGT!E70:BP70, "P")/(COUNTIF(DSGT!E70:BP70,"P")+COUNTIF(DSGT!E70:BP70,"A"))*100</f>
@@ -16702,7 +16688,7 @@
       </c>
       <c r="O68" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
@@ -16736,7 +16722,7 @@
       </c>
       <c r="I69" s="20">
         <f>COUNTIF(OOPM!E71:BP71, "P")/(COUNTIF(OOPM!E71:BP71,"P")+COUNTIF(OOPM!E71:BP71,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J69" s="20">
         <f>COUNTIF(DSGT!E71:BP71, "P")/(COUNTIF(DSGT!E71:BP71,"P")+COUNTIF(DSGT!E71:BP71,"A"))*100</f>
@@ -16760,7 +16746,7 @@
       </c>
       <c r="O69" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
@@ -16794,7 +16780,7 @@
       </c>
       <c r="I70" s="20">
         <f>COUNTIF(OOPM!E72:BP72, "P")/(COUNTIF(OOPM!E72:BP72,"P")+COUNTIF(OOPM!E72:BP72,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J70" s="20">
         <f>COUNTIF(DSGT!E72:BP72, "P")/(COUNTIF(DSGT!E72:BP72,"P")+COUNTIF(DSGT!E72:BP72,"A"))*100</f>
@@ -16818,7 +16804,7 @@
       </c>
       <c r="O70" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
@@ -16852,7 +16838,7 @@
       </c>
       <c r="I71" s="20">
         <f>COUNTIF(OOPM!E73:BP73, "P")/(COUNTIF(OOPM!E73:BP73,"P")+COUNTIF(OOPM!E73:BP73,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J71" s="20">
         <f>COUNTIF(DSGT!E73:BP73, "P")/(COUNTIF(DSGT!E73:BP73,"P")+COUNTIF(DSGT!E73:BP73,"A"))*100</f>
@@ -16876,7 +16862,7 @@
       </c>
       <c r="O71" s="27">
         <f t="shared" si="2"/>
-        <v>93.114035087719301</v>
+        <v>92.280701754385959</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
@@ -16910,7 +16896,7 @@
       </c>
       <c r="I72" s="20">
         <f>COUNTIF(OOPM!E74:BP74, "P")/(COUNTIF(OOPM!E74:BP74,"P")+COUNTIF(OOPM!E74:BP74,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J72" s="20">
         <f>COUNTIF(DSGT!E74:BP74, "P")/(COUNTIF(DSGT!E74:BP74,"P")+COUNTIF(DSGT!E74:BP74,"A"))*100</f>
@@ -16934,7 +16920,7 @@
       </c>
       <c r="O72" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
@@ -16968,7 +16954,7 @@
       </c>
       <c r="I73" s="20">
         <f>COUNTIF(OOPM!E75:BP75, "P")/(COUNTIF(OOPM!E75:BP75,"P")+COUNTIF(OOPM!E75:BP75,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J73" s="20">
         <f>COUNTIF(DSGT!E75:BP75, "P")/(COUNTIF(DSGT!E75:BP75,"P")+COUNTIF(DSGT!E75:BP75,"A"))*100</f>
@@ -16992,7 +16978,7 @@
       </c>
       <c r="O73" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
@@ -17026,7 +17012,7 @@
       </c>
       <c r="I74" s="20">
         <f>COUNTIF(OOPM!E76:BP76, "P")/(COUNTIF(OOPM!E76:BP76,"P")+COUNTIF(OOPM!E76:BP76,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J74" s="20">
         <f>COUNTIF(DSGT!E76:BP76, "P")/(COUNTIF(DSGT!E76:BP76,"P")+COUNTIF(DSGT!E76:BP76,"A"))*100</f>
@@ -17050,7 +17036,7 @@
       </c>
       <c r="O74" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
@@ -17084,7 +17070,7 @@
       </c>
       <c r="I75" s="20">
         <f>COUNTIF(OOPM!E77:BP77, "P")/(COUNTIF(OOPM!E77:BP77,"P")+COUNTIF(OOPM!E77:BP77,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J75" s="20">
         <f>COUNTIF(DSGT!E77:BP77, "P")/(COUNTIF(DSGT!E77:BP77,"P")+COUNTIF(DSGT!E77:BP77,"A"))*100</f>
@@ -17108,7 +17094,7 @@
       </c>
       <c r="O75" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
@@ -17142,7 +17128,7 @@
       </c>
       <c r="I76" s="20">
         <f>COUNTIF(OOPM!E78:BP78, "P")/(COUNTIF(OOPM!E78:BP78,"P")+COUNTIF(OOPM!E78:BP78,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J76" s="20">
         <f>COUNTIF(DSGT!E78:BP78, "P")/(COUNTIF(DSGT!E78:BP78,"P")+COUNTIF(DSGT!E78:BP78,"A"))*100</f>
@@ -17166,7 +17152,7 @@
       </c>
       <c r="O76" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
@@ -17200,7 +17186,7 @@
       </c>
       <c r="I77" s="20">
         <f>COUNTIF(OOPM!E79:BP79, "P")/(COUNTIF(OOPM!E79:BP79,"P")+COUNTIF(OOPM!E79:BP79,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J77" s="20">
         <f>COUNTIF(DSGT!E79:BP79, "P")/(COUNTIF(DSGT!E79:BP79,"P")+COUNTIF(DSGT!E79:BP79,"A"))*100</f>
@@ -17224,7 +17210,7 @@
       </c>
       <c r="O77" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
@@ -17258,7 +17244,7 @@
       </c>
       <c r="I78" s="20">
         <f>COUNTIF(OOPM!E80:BP80, "P")/(COUNTIF(OOPM!E80:BP80,"P")+COUNTIF(OOPM!E80:BP80,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J78" s="20">
         <f>COUNTIF(DSGT!E80:BP80, "P")/(COUNTIF(DSGT!E80:BP80,"P")+COUNTIF(DSGT!E80:BP80,"A"))*100</f>
@@ -17282,7 +17268,7 @@
       </c>
       <c r="O78" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
@@ -17316,7 +17302,7 @@
       </c>
       <c r="I79" s="20">
         <f>COUNTIF(OOPM!E81:BP81, "P")/(COUNTIF(OOPM!E81:BP81,"P")+COUNTIF(OOPM!E81:BP81,"A"))*100</f>
-        <v>25</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="J79" s="20">
         <f>COUNTIF(DSGT!E81:BP81, "P")/(COUNTIF(DSGT!E81:BP81,"P")+COUNTIF(DSGT!E81:BP81,"A"))*100</f>
@@ -17340,7 +17326,7 @@
       </c>
       <c r="O79" s="27">
         <f t="shared" si="2"/>
-        <v>28.114035087719298</v>
+        <v>28.94736842105263</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
@@ -17374,7 +17360,7 @@
       </c>
       <c r="I80" s="20">
         <f>COUNTIF(OOPM!E82:BP82, "P")/(COUNTIF(OOPM!E82:BP82,"P")+COUNTIF(OOPM!E82:BP82,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J80" s="20">
         <f>COUNTIF(DSGT!E82:BP82, "P")/(COUNTIF(DSGT!E82:BP82,"P")+COUNTIF(DSGT!E82:BP82,"A"))*100</f>
@@ -17398,7 +17384,7 @@
       </c>
       <c r="O80" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
@@ -17432,7 +17418,7 @@
       </c>
       <c r="I81" s="20">
         <f>COUNTIF(OOPM!E83:BP83, "P")/(COUNTIF(OOPM!E83:BP83,"P")+COUNTIF(OOPM!E83:BP83,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J81" s="20">
         <f>COUNTIF(DSGT!E83:BP83, "P")/(COUNTIF(DSGT!E83:BP83,"P")+COUNTIF(DSGT!E83:BP83,"A"))*100</f>
@@ -17456,7 +17442,7 @@
       </c>
       <c r="O81" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.3">
@@ -17490,7 +17476,7 @@
       </c>
       <c r="I82" s="20">
         <f>COUNTIF(OOPM!E84:BP84, "P")/(COUNTIF(OOPM!E84:BP84,"P")+COUNTIF(OOPM!E84:BP84,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J82" s="20">
         <f>COUNTIF(DSGT!E84:BP84, "P")/(COUNTIF(DSGT!E84:BP84,"P")+COUNTIF(DSGT!E84:BP84,"A"))*100</f>
@@ -17514,7 +17500,7 @@
       </c>
       <c r="O82" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.3">
@@ -17548,7 +17534,7 @@
       </c>
       <c r="I83" s="20">
         <f>COUNTIF(OOPM!E85:BP85, "P")/(COUNTIF(OOPM!E85:BP85,"P")+COUNTIF(OOPM!E85:BP85,"A"))*100</f>
-        <v>75</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="J83" s="20">
         <f>COUNTIF(DSGT!E85:BP85, "P")/(COUNTIF(DSGT!E85:BP85,"P")+COUNTIF(DSGT!E85:BP85,"A"))*100</f>
@@ -17572,12 +17558,12 @@
       </c>
       <c r="O83" s="27">
         <f t="shared" si="2"/>
-        <v>96.44736842105263</v>
+        <v>95.614035087719301</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:N83">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>75</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21764,18 +21750,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26129,18 +26115,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30158,18 +30144,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34184,18 +34170,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38378,18 +38364,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38401,7 +38387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="E7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -38475,11 +38461,12 @@
       <c r="H2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="17">
-        <f>COUNTIF(OOPM!E4:BP4,"P")/COUNTIF(OOPM!E4:BP4,"A")*100</f>
-        <v>33.333333333333329</v>
-      </c>
-      <c r="J2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>205</v>
+      </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
@@ -38531,8 +38518,12 @@
       <c r="H3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
@@ -38584,8 +38575,12 @@
       <c r="H4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="I4" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
@@ -38637,8 +38632,12 @@
       <c r="H5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
+      <c r="I5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
       <c r="M5" s="20"/>
@@ -38690,8 +38689,12 @@
       <c r="H6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
+      <c r="I6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
@@ -38743,8 +38746,12 @@
       <c r="H7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
+      <c r="I7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
@@ -38796,8 +38803,12 @@
       <c r="H8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
+      <c r="I8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
@@ -38849,8 +38860,12 @@
       <c r="H9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
+      <c r="I9" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
@@ -38902,8 +38917,12 @@
       <c r="H10" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
+      <c r="I10" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
@@ -38955,8 +38974,12 @@
       <c r="H11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
+      <c r="I11" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
@@ -39008,8 +39031,12 @@
       <c r="H12" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
+      <c r="I12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
@@ -39061,8 +39088,12 @@
       <c r="H13" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
+      <c r="I13" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
@@ -39114,8 +39145,12 @@
       <c r="H14" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
+      <c r="I14" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
@@ -39167,8 +39202,12 @@
       <c r="H15" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
+      <c r="I15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
@@ -39220,8 +39259,12 @@
       <c r="H16" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
+      <c r="I16" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
@@ -39273,8 +39316,12 @@
       <c r="H17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
+      <c r="I17" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
       <c r="M17" s="20"/>
@@ -39326,8 +39373,12 @@
       <c r="H18" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
+      <c r="I18" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
@@ -39379,8 +39430,12 @@
       <c r="H19" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
+      <c r="I19" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
@@ -39432,8 +39487,12 @@
       <c r="H20" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
+      <c r="I20" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -39485,8 +39544,12 @@
       <c r="H21" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
+      <c r="I21" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
@@ -39538,8 +39601,12 @@
       <c r="H22" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
+      <c r="I22" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
@@ -39591,8 +39658,12 @@
       <c r="H23" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
+      <c r="I23" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
@@ -39644,8 +39715,12 @@
       <c r="H24" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
+      <c r="I24" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
@@ -39697,8 +39772,12 @@
       <c r="H25" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
+      <c r="I25" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
@@ -39750,8 +39829,12 @@
       <c r="H26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
+      <c r="I26" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
@@ -39803,8 +39886,12 @@
       <c r="H27" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
+      <c r="I27" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
@@ -39856,8 +39943,12 @@
       <c r="H28" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
+      <c r="I28" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
@@ -39909,8 +40000,12 @@
       <c r="H29" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
+      <c r="I29" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
@@ -39962,8 +40057,12 @@
       <c r="H30" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="I30" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J30" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K30" s="20"/>
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
@@ -40015,8 +40114,12 @@
       <c r="H31" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="I31" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J31" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
@@ -40068,8 +40171,12 @@
       <c r="H32" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
+      <c r="I32" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
@@ -40121,8 +40228,12 @@
       <c r="H33" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
+      <c r="I33" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J33" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
@@ -40174,8 +40285,12 @@
       <c r="H34" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
+      <c r="I34" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J34" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
@@ -40227,8 +40342,12 @@
       <c r="H35" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
+      <c r="I35" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J35" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
       <c r="M35" s="20"/>
@@ -40280,8 +40399,12 @@
       <c r="H36" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
+      <c r="I36" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J36" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
@@ -40333,8 +40456,12 @@
       <c r="H37" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
+      <c r="I37" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J37" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
       <c r="M37" s="20"/>
@@ -40386,8 +40513,12 @@
       <c r="H38" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
+      <c r="I38" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J38" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K38" s="20"/>
       <c r="L38" s="20"/>
       <c r="M38" s="20"/>
@@ -40439,8 +40570,12 @@
       <c r="H39" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
+      <c r="I39" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
       <c r="M39" s="20"/>
@@ -40492,8 +40627,12 @@
       <c r="H40" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
+      <c r="I40" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J40" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
       <c r="M40" s="20"/>
@@ -40545,8 +40684,12 @@
       <c r="H41" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
+      <c r="I41" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J41" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K41" s="20"/>
       <c r="L41" s="20"/>
       <c r="M41" s="20"/>
@@ -40598,8 +40741,12 @@
       <c r="H42" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
+      <c r="I42" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J42" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
       <c r="M42" s="20"/>
@@ -40651,8 +40798,12 @@
       <c r="H43" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
+      <c r="I43" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J43" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K43" s="20"/>
       <c r="L43" s="20"/>
       <c r="M43" s="20"/>
@@ -40704,8 +40855,12 @@
       <c r="H44" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
+      <c r="I44" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J44" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K44" s="20"/>
       <c r="L44" s="20"/>
       <c r="M44" s="20"/>
@@ -40757,8 +40912,12 @@
       <c r="H45" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
+      <c r="I45" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J45" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K45" s="20"/>
       <c r="L45" s="20"/>
       <c r="M45" s="20"/>
@@ -40810,8 +40969,12 @@
       <c r="H46" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
+      <c r="I46" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J46" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K46" s="20"/>
       <c r="L46" s="20"/>
       <c r="M46" s="20"/>
@@ -40863,8 +41026,12 @@
       <c r="H47" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
+      <c r="I47" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J47" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K47" s="20"/>
       <c r="L47" s="20"/>
       <c r="M47" s="20"/>
@@ -40916,8 +41083,12 @@
       <c r="H48" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
+      <c r="I48" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J48" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K48" s="20"/>
       <c r="L48" s="20"/>
       <c r="M48" s="20"/>
@@ -40969,8 +41140,12 @@
       <c r="H49" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
+      <c r="I49" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J49" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K49" s="20"/>
       <c r="L49" s="20"/>
       <c r="M49" s="20"/>
@@ -41022,8 +41197,12 @@
       <c r="H50" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
+      <c r="I50" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J50" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K50" s="20"/>
       <c r="L50" s="20"/>
       <c r="M50" s="20"/>
@@ -41075,8 +41254,12 @@
       <c r="H51" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
+      <c r="I51" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J51" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K51" s="20"/>
       <c r="L51" s="20"/>
       <c r="M51" s="20"/>
@@ -41128,8 +41311,12 @@
       <c r="H52" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
+      <c r="I52" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J52" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K52" s="20"/>
       <c r="L52" s="20"/>
       <c r="M52" s="20"/>
@@ -41181,8 +41368,12 @@
       <c r="H53" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I53" s="20"/>
-      <c r="J53" s="20"/>
+      <c r="I53" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J53" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K53" s="20"/>
       <c r="L53" s="20"/>
       <c r="M53" s="20"/>
@@ -41234,8 +41425,12 @@
       <c r="H54" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
+      <c r="I54" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J54" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K54" s="20"/>
       <c r="L54" s="20"/>
       <c r="M54" s="20"/>
@@ -41287,8 +41482,12 @@
       <c r="H55" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
+      <c r="I55" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J55" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K55" s="20"/>
       <c r="L55" s="20"/>
       <c r="M55" s="20"/>
@@ -41340,8 +41539,12 @@
       <c r="H56" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
+      <c r="I56" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J56" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K56" s="20"/>
       <c r="L56" s="20"/>
       <c r="M56" s="20"/>
@@ -41393,8 +41596,12 @@
       <c r="H57" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I57" s="20"/>
-      <c r="J57" s="20"/>
+      <c r="I57" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J57" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K57" s="20"/>
       <c r="L57" s="20"/>
       <c r="M57" s="20"/>
@@ -41446,8 +41653,12 @@
       <c r="H58" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I58" s="20"/>
-      <c r="J58" s="20"/>
+      <c r="I58" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J58" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K58" s="20"/>
       <c r="L58" s="20"/>
       <c r="M58" s="20"/>
@@ -41499,8 +41710,12 @@
       <c r="H59" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
+      <c r="I59" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J59" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K59" s="20"/>
       <c r="L59" s="20"/>
       <c r="M59" s="20"/>
@@ -41552,8 +41767,12 @@
       <c r="H60" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I60" s="20"/>
-      <c r="J60" s="20"/>
+      <c r="I60" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J60" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K60" s="20"/>
       <c r="L60" s="20"/>
       <c r="M60" s="20"/>
@@ -41605,8 +41824,12 @@
       <c r="H61" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I61" s="20"/>
-      <c r="J61" s="20"/>
+      <c r="I61" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J61" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K61" s="20"/>
       <c r="L61" s="20"/>
       <c r="M61" s="20"/>
@@ -41658,8 +41881,12 @@
       <c r="H62" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I62" s="20"/>
-      <c r="J62" s="20"/>
+      <c r="I62" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J62" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K62" s="20"/>
       <c r="L62" s="20"/>
       <c r="M62" s="20"/>
@@ -41711,8 +41938,12 @@
       <c r="H63" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I63" s="20"/>
-      <c r="J63" s="20"/>
+      <c r="I63" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J63" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K63" s="20"/>
       <c r="L63" s="20"/>
       <c r="M63" s="20"/>
@@ -41764,8 +41995,12 @@
       <c r="H64" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I64" s="20"/>
-      <c r="J64" s="20"/>
+      <c r="I64" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J64" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K64" s="20"/>
       <c r="L64" s="20"/>
       <c r="M64" s="20"/>
@@ -41817,8 +42052,12 @@
       <c r="H65" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I65" s="20"/>
-      <c r="J65" s="20"/>
+      <c r="I65" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J65" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K65" s="20"/>
       <c r="L65" s="20"/>
       <c r="M65" s="20"/>
@@ -41870,8 +42109,12 @@
       <c r="H66" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I66" s="20"/>
-      <c r="J66" s="20"/>
+      <c r="I66" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J66" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K66" s="20"/>
       <c r="L66" s="20"/>
       <c r="M66" s="20"/>
@@ -41923,8 +42166,12 @@
       <c r="H67" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I67" s="20"/>
-      <c r="J67" s="20"/>
+      <c r="I67" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J67" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K67" s="20"/>
       <c r="L67" s="20"/>
       <c r="M67" s="20"/>
@@ -41976,8 +42223,12 @@
       <c r="H68" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I68" s="20"/>
-      <c r="J68" s="20"/>
+      <c r="I68" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J68" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K68" s="20"/>
       <c r="L68" s="20"/>
       <c r="M68" s="20"/>
@@ -42029,8 +42280,12 @@
       <c r="H69" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I69" s="20"/>
-      <c r="J69" s="20"/>
+      <c r="I69" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J69" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K69" s="20"/>
       <c r="L69" s="20"/>
       <c r="M69" s="20"/>
@@ -42082,8 +42337,12 @@
       <c r="H70" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I70" s="20"/>
-      <c r="J70" s="20"/>
+      <c r="I70" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J70" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K70" s="20"/>
       <c r="L70" s="20"/>
       <c r="M70" s="20"/>
@@ -42135,8 +42394,12 @@
       <c r="H71" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I71" s="20"/>
-      <c r="J71" s="20"/>
+      <c r="I71" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J71" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K71" s="20"/>
       <c r="L71" s="20"/>
       <c r="M71" s="20"/>
@@ -42188,8 +42451,12 @@
       <c r="H72" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I72" s="20"/>
-      <c r="J72" s="20"/>
+      <c r="I72" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J72" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K72" s="20"/>
       <c r="L72" s="20"/>
       <c r="M72" s="20"/>
@@ -42241,8 +42508,12 @@
       <c r="H73" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I73" s="20"/>
-      <c r="J73" s="20"/>
+      <c r="I73" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J73" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K73" s="20"/>
       <c r="L73" s="20"/>
       <c r="M73" s="20"/>
@@ -42294,8 +42565,12 @@
       <c r="H74" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I74" s="20"/>
-      <c r="J74" s="20"/>
+      <c r="I74" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J74" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K74" s="20"/>
       <c r="L74" s="20"/>
       <c r="M74" s="20"/>
@@ -42347,8 +42622,12 @@
       <c r="H75" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I75" s="20"/>
-      <c r="J75" s="20"/>
+      <c r="I75" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J75" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K75" s="20"/>
       <c r="L75" s="20"/>
       <c r="M75" s="20"/>
@@ -42400,8 +42679,12 @@
       <c r="H76" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I76" s="20"/>
-      <c r="J76" s="20"/>
+      <c r="I76" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J76" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K76" s="20"/>
       <c r="L76" s="20"/>
       <c r="M76" s="20"/>
@@ -42453,8 +42736,12 @@
       <c r="H77" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I77" s="20"/>
-      <c r="J77" s="20"/>
+      <c r="I77" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J77" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K77" s="20"/>
       <c r="L77" s="20"/>
       <c r="M77" s="20"/>
@@ -42506,8 +42793,12 @@
       <c r="H78" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I78" s="20"/>
-      <c r="J78" s="20"/>
+      <c r="I78" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J78" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K78" s="20"/>
       <c r="L78" s="20"/>
       <c r="M78" s="20"/>
@@ -42559,8 +42850,12 @@
       <c r="H79" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I79" s="20"/>
-      <c r="J79" s="20"/>
+      <c r="I79" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J79" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K79" s="20"/>
       <c r="L79" s="20"/>
       <c r="M79" s="20"/>
@@ -42612,8 +42907,12 @@
       <c r="H80" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I80" s="20"/>
-      <c r="J80" s="20"/>
+      <c r="I80" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J80" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K80" s="20"/>
       <c r="L80" s="20"/>
       <c r="M80" s="20"/>
@@ -42665,8 +42964,12 @@
       <c r="H81" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I81" s="20"/>
-      <c r="J81" s="20"/>
+      <c r="I81" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J81" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K81" s="20"/>
       <c r="L81" s="20"/>
       <c r="M81" s="20"/>
@@ -42718,8 +43021,12 @@
       <c r="H82" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I82" s="20"/>
-      <c r="J82" s="20"/>
+      <c r="I82" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J82" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K82" s="20"/>
       <c r="L82" s="20"/>
       <c r="M82" s="20"/>
@@ -42771,8 +43078,12 @@
       <c r="H83" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I83" s="20"/>
-      <c r="J83" s="20"/>
+      <c r="I83" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J83" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K83" s="20"/>
       <c r="L83" s="20"/>
       <c r="M83" s="20"/>
@@ -42824,8 +43135,12 @@
       <c r="H84" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I84" s="20"/>
-      <c r="J84" s="20"/>
+      <c r="I84" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J84" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K84" s="20"/>
       <c r="L84" s="20"/>
       <c r="M84" s="20"/>
@@ -42877,8 +43192,12 @@
       <c r="H85" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I85" s="20"/>
-      <c r="J85" s="20"/>
+      <c r="I85" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J85" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="K85" s="20"/>
       <c r="L85" s="20"/>
       <c r="M85" s="20"/>
@@ -42915,18 +43234,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42955,7 +43274,7 @@
       <c r="C1" s="31"/>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -42967,7 +43286,7 @@
       <c r="M1" s="32"/>
       <c r="N1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
@@ -46944,18 +47263,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46981,7 +47300,7 @@
       <c r="C1" s="31"/>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -46993,7 +47312,7 @@
       <c r="M1" s="32"/>
       <c r="N1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
@@ -50970,18 +51289,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
email system added. everything almost done.
</commit_message>
<xml_diff>
--- a/workbooks/SE.xlsx
+++ b/workbooks/SE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EMIII" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5983" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6067" uniqueCount="219">
   <si>
     <t xml:space="preserve">Class/Sem : </t>
   </si>
@@ -46,18 +46,6 @@
     <t xml:space="preserve">Date: </t>
   </si>
   <si>
-    <t>25/08</t>
-  </si>
-  <si>
-    <t>14/09</t>
-  </si>
-  <si>
-    <t>26/08</t>
-  </si>
-  <si>
-    <t>01/08</t>
-  </si>
-  <si>
     <t>Roll No.</t>
   </si>
   <si>
@@ -70,13 +58,25 @@
     <t>Student name</t>
   </si>
   <si>
-    <t>Sun</t>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
   </si>
   <si>
     <t>Mon</t>
-  </si>
-  <si>
-    <t>Tue</t>
   </si>
   <si>
     <t>R-23-0336</t>
@@ -241,7 +241,7 @@
     <t>KALE ADWAIT VIVEK</t>
   </si>
   <si>
-    <t>R-22-0188</t>
+    <t>R-23-0188</t>
   </si>
   <si>
     <t>KALE ISHA PRAKASH</t>
@@ -583,6 +583,12 @@
     <t>KULKARNI YASH</t>
   </si>
   <si>
+    <t>25/08</t>
+  </si>
+  <si>
+    <t>01-10</t>
+  </si>
+  <si>
     <t>Name of Course : DLCOA</t>
   </si>
   <si>
@@ -592,7 +598,10 @@
     <t>1/8</t>
   </si>
   <si>
-    <t>Monday</t>
+    <t>01/08</t>
+  </si>
+  <si>
+    <t>26/08</t>
   </si>
   <si>
     <t>Name of Course : CG</t>
@@ -613,13 +622,22 @@
     <t>Name of Course Teacher : Prof. S.S. Athalye</t>
   </si>
   <si>
+    <t>Tue</t>
+  </si>
+  <si>
     <t>Name of Course : OOPM</t>
+  </si>
+  <si>
+    <t>14/09</t>
   </si>
   <si>
     <t>22/09</t>
   </si>
   <si>
     <t>23/09</t>
+  </si>
+  <si>
+    <t>Satuday</t>
   </si>
   <si>
     <t>Name of Course : DS LAB</t>
@@ -668,24 +686,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Satuday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
   </si>
 </sst>
 </file>
@@ -963,7 +963,57 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="46">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1652,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1787,76 +1837,76 @@
     </row>
     <row r="3" spans="1:35" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="F3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>187</v>
-      </c>
       <c r="I3" s="4" t="s">
-        <v>213</v>
+        <v>13</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>217</v>
+        <v>14</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>218</v>
+        <v>9</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>216</v>
+        <v>10</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>214</v>
+        <v>11</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>187</v>
+        <v>12</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>213</v>
+        <v>13</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>217</v>
+        <v>14</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>218</v>
+        <v>9</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>216</v>
+        <v>10</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>214</v>
+        <v>11</v>
       </c>
       <c r="T3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="V3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>217</v>
-      </c>
       <c r="W3" s="4" t="s">
-        <v>218</v>
+        <v>9</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>216</v>
+        <v>10</v>
       </c>
       <c r="Y3" s="4"/>
       <c r="Z3" s="5"/>
@@ -2427,16 +2477,16 @@
         <v>20</v>
       </c>
       <c r="P10" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q10" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R10" s="20" t="s">
         <v>20</v>
       </c>
       <c r="S10" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T10" s="20" t="s">
         <v>19</v>
@@ -2479,37 +2529,37 @@
         <v>35</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>20</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>20</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L11" s="20" t="s">
         <v>20</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N11" s="20" t="s">
         <v>20</v>
       </c>
       <c r="O11" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P11" s="20" t="s">
         <v>20</v>
@@ -2518,7 +2568,7 @@
         <v>20</v>
       </c>
       <c r="R11" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S11" s="20" t="s">
         <v>20</v>
@@ -8850,23 +8900,23 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -8874,8 +8924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8891,7 +8941,7 @@
       <c r="C1" s="31"/>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -8903,7 +8953,7 @@
       <c r="M1" s="32"/>
       <c r="N1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
@@ -8936,7 +8986,7 @@
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
@@ -8971,19 +9021,19 @@
     </row>
     <row r="3" spans="1:35" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>187</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -10205,7 +10255,7 @@
         <v>71</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
@@ -10252,7 +10302,7 @@
         <v>73</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
@@ -12880,18 +12930,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12904,7 +12954,7 @@
   <dimension ref="A1:O83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I85" sqref="I85"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12919,49 +12969,49 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -13041,7 +13091,7 @@
       </c>
       <c r="F3" s="20">
         <f>COUNTIF(DS!E5:BP5, "P")/(COUNTIF(DS!E5:BP5,"P")+COUNTIF(DS!E5:BP5,"A"))*100</f>
-        <v>100</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="G3" s="20">
         <f>COUNTIF(DLCOA!E5:BP5, "P")/(COUNTIF(DLCOA!E5:BP5,"P")+COUNTIF(DLCOA!E5:BP5,"A"))*100</f>
@@ -13077,7 +13127,7 @@
       </c>
       <c r="O3" s="27">
         <f t="shared" si="0"/>
-        <v>19.333333333333332</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -13099,7 +13149,7 @@
       </c>
       <c r="F4" s="20">
         <f>COUNTIF(DS!E6:BP6, "P")/(COUNTIF(DS!E6:BP6,"P")+COUNTIF(DS!E6:BP6,"A"))*100</f>
-        <v>100</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="G4" s="20">
         <f>COUNTIF(DLCOA!E6:BP6, "P")/(COUNTIF(DLCOA!E6:BP6,"P")+COUNTIF(DLCOA!E6:BP6,"A"))*100</f>
@@ -13135,7 +13185,7 @@
       </c>
       <c r="O4" s="27">
         <f t="shared" si="0"/>
-        <v>90.333333333333329</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -13157,7 +13207,7 @@
       </c>
       <c r="F5" s="20">
         <f>COUNTIF(DS!E7:BP7, "P")/(COUNTIF(DS!E7:BP7,"P")+COUNTIF(DS!E7:BP7,"A"))*100</f>
-        <v>100</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="G5" s="20">
         <f>COUNTIF(DLCOA!E7:BP7, "P")/(COUNTIF(DLCOA!E7:BP7,"P")+COUNTIF(DLCOA!E7:BP7,"A"))*100</f>
@@ -13193,7 +13243,7 @@
       </c>
       <c r="O5" s="27">
         <f t="shared" si="0"/>
-        <v>91.333333333333329</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -13215,7 +13265,7 @@
       </c>
       <c r="F6" s="20">
         <f>COUNTIF(DS!E8:BP8, "P")/(COUNTIF(DS!E8:BP8,"P")+COUNTIF(DS!E8:BP8,"A"))*100</f>
-        <v>50</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="G6" s="20">
         <f>COUNTIF(DLCOA!E8:BP8, "P")/(COUNTIF(DLCOA!E8:BP8,"P")+COUNTIF(DLCOA!E8:BP8,"A"))*100</f>
@@ -13251,7 +13301,7 @@
       </c>
       <c r="O6" s="27">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>85.333333333333343</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -13273,7 +13323,7 @@
       </c>
       <c r="F7" s="20">
         <f>COUNTIF(DS!E9:BP9, "P")/(COUNTIF(DS!E9:BP9,"P")+COUNTIF(DS!E9:BP9,"A"))*100</f>
-        <v>100</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="G7" s="20">
         <f>COUNTIF(DLCOA!E9:BP9, "P")/(COUNTIF(DLCOA!E9:BP9,"P")+COUNTIF(DLCOA!E9:BP9,"A"))*100</f>
@@ -13309,7 +13359,7 @@
       </c>
       <c r="O7" s="27">
         <f t="shared" si="0"/>
-        <v>96.833333333333343</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -13327,11 +13377,11 @@
       </c>
       <c r="E8" s="20">
         <f>COUNTIF(EMIII!E10:BP10, "P")/(COUNTIF(EMIII!E10:BP10,"P")+COUNTIF(EMIII!E10:BP10,"A"))*100</f>
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F8" s="20">
         <f>COUNTIF(DS!E10:BP10, "P")/(COUNTIF(DS!E10:BP10,"P")+COUNTIF(DS!E10:BP10,"A"))*100</f>
-        <v>100</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="G8" s="20">
         <f>COUNTIF(DLCOA!E10:BP10, "P")/(COUNTIF(DLCOA!E10:BP10,"P")+COUNTIF(DLCOA!E10:BP10,"A"))*100</f>
@@ -13347,7 +13397,7 @@
       </c>
       <c r="J8" s="20">
         <f>COUNTIF(DSGT!E10:BP10, "P")/(COUNTIF(DSGT!E10:BP10,"P")+COUNTIF(DSGT!E10:BP10,"A"))*100</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K8" s="20">
         <f>COUNTIF(OOPMLAB!E10:BP10, "P")/(COUNTIF(OOPMLAB!E10:BP10,"P")+COUNTIF(OOPMLAB!E10:BP10,"A"))*100</f>
@@ -13367,7 +13417,7 @@
       </c>
       <c r="O8" s="27">
         <f t="shared" si="0"/>
-        <v>84.166666666666657</v>
+        <v>69.333333333333329</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -13385,11 +13435,11 @@
       </c>
       <c r="E9" s="20">
         <f>COUNTIF(EMIII!E11:BP11, "P")/(COUNTIF(EMIII!E11:BP11,"P")+COUNTIF(EMIII!E11:BP11,"A"))*100</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="F9" s="20">
         <f>COUNTIF(DS!E11:BP11, "P")/(COUNTIF(DS!E11:BP11,"P")+COUNTIF(DS!E11:BP11,"A"))*100</f>
-        <v>100</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="G9" s="20">
         <f>COUNTIF(DLCOA!E11:BP11, "P")/(COUNTIF(DLCOA!E11:BP11,"P")+COUNTIF(DLCOA!E11:BP11,"A"))*100</f>
@@ -13405,7 +13455,7 @@
       </c>
       <c r="J9" s="20">
         <f>COUNTIF(DSGT!E11:BP11, "P")/(COUNTIF(DSGT!E11:BP11,"P")+COUNTIF(DSGT!E11:BP11,"A"))*100</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K9" s="20">
         <f>COUNTIF(OOPMLAB!E11:BP11, "P")/(COUNTIF(OOPMLAB!E11:BP11,"P")+COUNTIF(OOPMLAB!E11:BP11,"A"))*100</f>
@@ -13417,7 +13467,7 @@
       </c>
       <c r="M9" s="20">
         <f>COUNTIF(CGLAB!E11:BP11, "P")/(COUNTIF(CGLAB!E11:BP11,"P")+COUNTIF(CGLAB!E11:BP11,"A"))*100</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N9" s="20">
         <f>COUNTIF(DLCOALAB!E11:BP11, "P")/(COUNTIF(DLCOALAB!E11:BP11,"P")+COUNTIF(DLCOALAB!E11:BP11,"A"))*100</f>
@@ -13425,7 +13475,7 @@
       </c>
       <c r="O9" s="27">
         <f t="shared" si="0"/>
-        <v>95.166666666666657</v>
+        <v>68.333333333333329</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -13505,7 +13555,7 @@
       </c>
       <c r="F11" s="20">
         <f>COUNTIF(DS!E13:BP13, "P")/(COUNTIF(DS!E13:BP13,"P")+COUNTIF(DS!E13:BP13,"A"))*100</f>
-        <v>50</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="G11" s="20">
         <f>COUNTIF(DLCOA!E13:BP13, "P")/(COUNTIF(DLCOA!E13:BP13,"P")+COUNTIF(DLCOA!E13:BP13,"A"))*100</f>
@@ -13541,7 +13591,7 @@
       </c>
       <c r="O11" s="27">
         <f t="shared" si="0"/>
-        <v>89.666666666666657</v>
+        <v>91.333333333333329</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -13737,7 +13787,7 @@
       </c>
       <c r="F15" s="20">
         <f>COUNTIF(DS!E17:BP17, "P")/(COUNTIF(DS!E17:BP17,"P")+COUNTIF(DS!E17:BP17,"A"))*100</f>
-        <v>50</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="G15" s="20">
         <f>COUNTIF(DLCOA!E17:BP17, "P")/(COUNTIF(DLCOA!E17:BP17,"P")+COUNTIF(DLCOA!E17:BP17,"A"))*100</f>
@@ -13773,7 +13823,7 @@
       </c>
       <c r="O15" s="27">
         <f t="shared" si="0"/>
-        <v>90.666666666666657</v>
+        <v>92.333333333333329</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -13853,7 +13903,7 @@
       </c>
       <c r="F17" s="20">
         <f>COUNTIF(DS!E19:BP19, "P")/(COUNTIF(DS!E19:BP19,"P")+COUNTIF(DS!E19:BP19,"A"))*100</f>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="G17" s="20">
         <f>COUNTIF(DLCOA!E19:BP19, "P")/(COUNTIF(DLCOA!E19:BP19,"P")+COUNTIF(DLCOA!E19:BP19,"A"))*100</f>
@@ -13889,7 +13939,7 @@
       </c>
       <c r="O17" s="27">
         <f t="shared" si="0"/>
-        <v>85.666666666666657</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -14085,7 +14135,7 @@
       </c>
       <c r="F21" s="20">
         <f>COUNTIF(DS!E23:BP23, "P")/(COUNTIF(DS!E23:BP23,"P")+COUNTIF(DS!E23:BP23,"A"))*100</f>
-        <v>50</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="G21" s="20">
         <f>COUNTIF(DLCOA!E23:BP23, "P")/(COUNTIF(DLCOA!E23:BP23,"P")+COUNTIF(DLCOA!E23:BP23,"A"))*100</f>
@@ -14121,7 +14171,7 @@
       </c>
       <c r="O21" s="27">
         <f t="shared" si="0"/>
-        <v>90.166666666666657</v>
+        <v>91.833333333333329</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -14433,7 +14483,7 @@
       </c>
       <c r="F27" s="20">
         <f>COUNTIF(DS!E29:BP29, "P")/(COUNTIF(DS!E29:BP29,"P")+COUNTIF(DS!E29:BP29,"A"))*100</f>
-        <v>50</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="G27" s="20">
         <f>COUNTIF(DLCOA!E29:BP29, "P")/(COUNTIF(DLCOA!E29:BP29,"P")+COUNTIF(DLCOA!E29:BP29,"A"))*100</f>
@@ -14453,7 +14503,7 @@
       </c>
       <c r="K27" s="20">
         <f>COUNTIF(OOPMLAB!E29:BP29, "P")/(COUNTIF(OOPMLAB!E29:BP29,"P")+COUNTIF(OOPMLAB!E29:BP29,"A"))*100</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L27" s="20">
         <f>COUNTIF(DSLAB!E29:BP29, "P")/(COUNTIF(DSLAB!E29:BP29,"P")+COUNTIF(DSLAB!E29:BP29,"A"))*100</f>
@@ -14461,15 +14511,15 @@
       </c>
       <c r="M27" s="20">
         <f>COUNTIF(CGLAB!E29:BP29, "P")/(COUNTIF(CGLAB!E29:BP29,"P")+COUNTIF(CGLAB!E29:BP29,"A"))*100</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N27" s="20">
         <f>COUNTIF(DLCOALAB!E29:BP29, "P")/(COUNTIF(DLCOALAB!E29:BP29,"P")+COUNTIF(DLCOALAB!E29:BP29,"A"))*100</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O27" s="27">
         <f t="shared" si="0"/>
-        <v>90.666666666666657</v>
+        <v>62.333333333333329</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -14519,15 +14569,15 @@
       </c>
       <c r="M28" s="20">
         <f>COUNTIF(CGLAB!E30:BP30, "P")/(COUNTIF(CGLAB!E30:BP30,"P")+COUNTIF(CGLAB!E30:BP30,"A"))*100</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N28" s="20">
         <f>COUNTIF(DLCOALAB!E30:BP30, "P")/(COUNTIF(DLCOALAB!E30:BP30,"P")+COUNTIF(DLCOALAB!E30:BP30,"A"))*100</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O28" s="27">
         <f t="shared" si="0"/>
-        <v>95.666666666666657</v>
+        <v>75.666666666666657</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -17722,7 +17772,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:N83">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+      <formula>75</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O83">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+      <formula>75</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+      <formula>75</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O28">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+      <formula>75</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>75</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>75</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17735,8 +17806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="A1:AI85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17797,12 +17868,14 @@
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>184</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1"/>
+        <v>184</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -17834,24 +17907,26 @@
     </row>
     <row r="3" spans="1:35" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="13"/>
+        <v>12</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="H3" s="14"/>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
@@ -17900,7 +17975,9 @@
       <c r="F4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="H4" s="15"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -17949,7 +18026,9 @@
       <c r="F5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="16"/>
+      <c r="G5" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="H5" s="16"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
@@ -17998,7 +18077,9 @@
       <c r="F6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="H6" s="16"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
@@ -18047,7 +18128,9 @@
       <c r="F7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="16"/>
+      <c r="G7" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="H7" s="16"/>
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
@@ -18096,7 +18179,9 @@
       <c r="F8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="16"/>
+      <c r="G8" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="H8" s="16"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
@@ -18145,7 +18230,9 @@
       <c r="F9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="16"/>
+      <c r="G9" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="H9" s="16"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
@@ -18194,7 +18281,9 @@
       <c r="F10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="H10" s="16"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
@@ -18243,7 +18332,9 @@
       <c r="F11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="16"/>
+      <c r="G11" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="H11" s="16"/>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
@@ -18292,7 +18383,9 @@
       <c r="F12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="16"/>
+      <c r="G12" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H12" s="16"/>
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
@@ -18341,7 +18434,9 @@
       <c r="F13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="16"/>
+      <c r="G13" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H13" s="16"/>
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
@@ -18390,7 +18485,9 @@
       <c r="F14" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="16"/>
+      <c r="G14" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H14" s="16"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -18439,7 +18536,9 @@
       <c r="F15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="16"/>
+      <c r="G15" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H15" s="16"/>
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
@@ -18488,7 +18587,9 @@
       <c r="F16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="16"/>
+      <c r="G16" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H16" s="16"/>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
@@ -18537,7 +18638,9 @@
       <c r="F17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="16"/>
+      <c r="G17" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H17" s="16"/>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
@@ -18586,7 +18689,9 @@
       <c r="F18" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="16"/>
+      <c r="G18" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H18" s="16"/>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
@@ -18635,7 +18740,9 @@
       <c r="F19" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="16"/>
+      <c r="G19" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H19" s="16"/>
       <c r="I19" s="20"/>
       <c r="J19" s="20"/>
@@ -18684,7 +18791,9 @@
       <c r="F20" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="16"/>
+      <c r="G20" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H20" s="16"/>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
@@ -18733,7 +18842,9 @@
       <c r="F21" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="16"/>
+      <c r="G21" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H21" s="16"/>
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
@@ -18782,7 +18893,9 @@
       <c r="F22" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="16"/>
+      <c r="G22" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H22" s="16"/>
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
@@ -18831,7 +18944,9 @@
       <c r="F23" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="16"/>
+      <c r="G23" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H23" s="16"/>
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
@@ -18880,7 +18995,9 @@
       <c r="F24" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="16"/>
+      <c r="G24" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H24" s="16"/>
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
@@ -18929,7 +19046,9 @@
       <c r="F25" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="16"/>
+      <c r="G25" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H25" s="16"/>
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
@@ -18978,7 +19097,9 @@
       <c r="F26" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="16"/>
+      <c r="G26" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H26" s="16"/>
       <c r="I26" s="20"/>
       <c r="J26" s="20"/>
@@ -19027,7 +19148,9 @@
       <c r="F27" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="16"/>
+      <c r="G27" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H27" s="16"/>
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
@@ -19076,7 +19199,9 @@
       <c r="F28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="16"/>
+      <c r="G28" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H28" s="16"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
@@ -19125,7 +19250,9 @@
       <c r="F29" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="16"/>
+      <c r="G29" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H29" s="16"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
@@ -19174,7 +19301,9 @@
       <c r="F30" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="16"/>
+      <c r="G30" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H30" s="16"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -19223,7 +19352,9 @@
       <c r="F31" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="16"/>
+      <c r="G31" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H31" s="16"/>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
@@ -19272,7 +19403,9 @@
       <c r="F32" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="16"/>
+      <c r="G32" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H32" s="16"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -19321,7 +19454,9 @@
       <c r="F33" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="16"/>
+      <c r="G33" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H33" s="16"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
@@ -19370,7 +19505,9 @@
       <c r="F34" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="16"/>
+      <c r="G34" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H34" s="16"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
@@ -19419,7 +19556,9 @@
       <c r="F35" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G35" s="16"/>
+      <c r="G35" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H35" s="16"/>
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
@@ -19468,7 +19607,9 @@
       <c r="F36" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="16"/>
+      <c r="G36" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H36" s="16"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
@@ -19517,7 +19658,9 @@
       <c r="F37" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G37" s="16"/>
+      <c r="G37" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H37" s="16"/>
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
@@ -19566,7 +19709,9 @@
       <c r="F38" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G38" s="16"/>
+      <c r="G38" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H38" s="16"/>
       <c r="I38" s="20"/>
       <c r="J38" s="20"/>
@@ -19615,7 +19760,9 @@
       <c r="F39" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G39" s="16"/>
+      <c r="G39" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H39" s="16"/>
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
@@ -19664,7 +19811,9 @@
       <c r="F40" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="16"/>
+      <c r="G40" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H40" s="16"/>
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
@@ -19713,7 +19862,9 @@
       <c r="F41" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G41" s="16"/>
+      <c r="G41" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H41" s="16"/>
       <c r="I41" s="20"/>
       <c r="J41" s="20"/>
@@ -19762,7 +19913,9 @@
       <c r="F42" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="16"/>
+      <c r="G42" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H42" s="16"/>
       <c r="I42" s="20"/>
       <c r="J42" s="20"/>
@@ -19811,7 +19964,9 @@
       <c r="F43" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G43" s="16"/>
+      <c r="G43" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H43" s="16"/>
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
@@ -19860,7 +20015,9 @@
       <c r="F44" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G44" s="16"/>
+      <c r="G44" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H44" s="16"/>
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
@@ -19909,7 +20066,9 @@
       <c r="F45" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G45" s="16"/>
+      <c r="G45" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H45" s="16"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
@@ -19958,7 +20117,9 @@
       <c r="F46" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="16"/>
+      <c r="G46" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H46" s="16"/>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
@@ -20007,7 +20168,9 @@
       <c r="F47" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G47" s="16"/>
+      <c r="G47" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H47" s="16"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
@@ -20056,7 +20219,9 @@
       <c r="F48" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G48" s="16"/>
+      <c r="G48" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H48" s="16"/>
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
@@ -20105,7 +20270,9 @@
       <c r="F49" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G49" s="16"/>
+      <c r="G49" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H49" s="16"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
@@ -20154,7 +20321,9 @@
       <c r="F50" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G50" s="16"/>
+      <c r="G50" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H50" s="16"/>
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
@@ -20203,7 +20372,9 @@
       <c r="F51" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G51" s="16"/>
+      <c r="G51" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H51" s="16"/>
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
@@ -20252,7 +20423,9 @@
       <c r="F52" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G52" s="16"/>
+      <c r="G52" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H52" s="16"/>
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
@@ -20301,7 +20474,9 @@
       <c r="F53" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G53" s="16"/>
+      <c r="G53" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H53" s="16"/>
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
@@ -20350,7 +20525,9 @@
       <c r="F54" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G54" s="16"/>
+      <c r="G54" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H54" s="16"/>
       <c r="I54" s="20"/>
       <c r="J54" s="20"/>
@@ -20399,7 +20576,9 @@
       <c r="F55" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G55" s="16"/>
+      <c r="G55" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H55" s="16"/>
       <c r="I55" s="20"/>
       <c r="J55" s="20"/>
@@ -20448,7 +20627,9 @@
       <c r="F56" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G56" s="16"/>
+      <c r="G56" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H56" s="16"/>
       <c r="I56" s="20"/>
       <c r="J56" s="20"/>
@@ -20497,7 +20678,9 @@
       <c r="F57" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G57" s="16"/>
+      <c r="G57" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H57" s="16"/>
       <c r="I57" s="20"/>
       <c r="J57" s="20"/>
@@ -20546,7 +20729,9 @@
       <c r="F58" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G58" s="16"/>
+      <c r="G58" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H58" s="16"/>
       <c r="I58" s="20"/>
       <c r="J58" s="20"/>
@@ -20595,7 +20780,9 @@
       <c r="F59" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G59" s="16"/>
+      <c r="G59" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H59" s="16"/>
       <c r="I59" s="20"/>
       <c r="J59" s="20"/>
@@ -20644,7 +20831,9 @@
       <c r="F60" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G60" s="16"/>
+      <c r="G60" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H60" s="16"/>
       <c r="I60" s="20"/>
       <c r="J60" s="20"/>
@@ -20693,7 +20882,9 @@
       <c r="F61" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G61" s="16"/>
+      <c r="G61" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H61" s="16"/>
       <c r="I61" s="20"/>
       <c r="J61" s="20"/>
@@ -20742,7 +20933,9 @@
       <c r="F62" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G62" s="16"/>
+      <c r="G62" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H62" s="16"/>
       <c r="I62" s="20"/>
       <c r="J62" s="20"/>
@@ -20791,7 +20984,9 @@
       <c r="F63" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G63" s="16"/>
+      <c r="G63" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H63" s="16"/>
       <c r="I63" s="20"/>
       <c r="J63" s="20"/>
@@ -20840,7 +21035,9 @@
       <c r="F64" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G64" s="16"/>
+      <c r="G64" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H64" s="16"/>
       <c r="I64" s="20"/>
       <c r="J64" s="20"/>
@@ -20889,7 +21086,9 @@
       <c r="F65" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G65" s="16"/>
+      <c r="G65" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H65" s="16"/>
       <c r="I65" s="20"/>
       <c r="J65" s="20"/>
@@ -20938,7 +21137,9 @@
       <c r="F66" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G66" s="16"/>
+      <c r="G66" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H66" s="16"/>
       <c r="I66" s="20"/>
       <c r="J66" s="20"/>
@@ -20987,7 +21188,9 @@
       <c r="F67" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G67" s="16"/>
+      <c r="G67" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H67" s="16"/>
       <c r="I67" s="20"/>
       <c r="J67" s="20"/>
@@ -21036,7 +21239,9 @@
       <c r="F68" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G68" s="16"/>
+      <c r="G68" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H68" s="16"/>
       <c r="I68" s="20"/>
       <c r="J68" s="20"/>
@@ -21085,7 +21290,9 @@
       <c r="F69" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G69" s="16"/>
+      <c r="G69" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H69" s="16"/>
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
@@ -21134,7 +21341,9 @@
       <c r="F70" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G70" s="16"/>
+      <c r="G70" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H70" s="16"/>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
@@ -21183,7 +21392,9 @@
       <c r="F71" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G71" s="16"/>
+      <c r="G71" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H71" s="16"/>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
@@ -21232,7 +21443,9 @@
       <c r="F72" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G72" s="16"/>
+      <c r="G72" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H72" s="16"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
@@ -21281,7 +21494,9 @@
       <c r="F73" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G73" s="16"/>
+      <c r="G73" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H73" s="16"/>
       <c r="I73" s="20"/>
       <c r="J73" s="20"/>
@@ -21330,7 +21545,9 @@
       <c r="F74" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G74" s="16"/>
+      <c r="G74" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H74" s="16"/>
       <c r="I74" s="20"/>
       <c r="J74" s="20"/>
@@ -21379,7 +21596,9 @@
       <c r="F75" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G75" s="16"/>
+      <c r="G75" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H75" s="16"/>
       <c r="I75" s="20"/>
       <c r="J75" s="20"/>
@@ -21428,7 +21647,9 @@
       <c r="F76" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G76" s="16"/>
+      <c r="G76" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H76" s="16"/>
       <c r="I76" s="20"/>
       <c r="J76" s="20"/>
@@ -21477,7 +21698,9 @@
       <c r="F77" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G77" s="16"/>
+      <c r="G77" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H77" s="16"/>
       <c r="I77" s="20"/>
       <c r="J77" s="20"/>
@@ -21526,7 +21749,9 @@
       <c r="F78" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G78" s="16"/>
+      <c r="G78" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H78" s="16"/>
       <c r="I78" s="20"/>
       <c r="J78" s="20"/>
@@ -21575,7 +21800,9 @@
       <c r="F79" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G79" s="16"/>
+      <c r="G79" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H79" s="16"/>
       <c r="I79" s="20"/>
       <c r="J79" s="20"/>
@@ -21624,7 +21851,9 @@
       <c r="F80" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G80" s="16"/>
+      <c r="G80" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H80" s="16"/>
       <c r="I80" s="20"/>
       <c r="J80" s="20"/>
@@ -21673,7 +21902,9 @@
       <c r="F81" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G81" s="16"/>
+      <c r="G81" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H81" s="16"/>
       <c r="I81" s="20"/>
       <c r="J81" s="20"/>
@@ -21722,7 +21953,9 @@
       <c r="F82" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G82" s="16"/>
+      <c r="G82" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H82" s="16"/>
       <c r="I82" s="20"/>
       <c r="J82" s="20"/>
@@ -21771,7 +22004,9 @@
       <c r="F83" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G83" s="16"/>
+      <c r="G83" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H83" s="16"/>
       <c r="I83" s="20"/>
       <c r="J83" s="20"/>
@@ -21820,7 +22055,9 @@
       <c r="F84" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G84" s="16"/>
+      <c r="G84" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H84" s="16"/>
       <c r="I84" s="20"/>
       <c r="J84" s="20"/>
@@ -21869,7 +22106,9 @@
       <c r="F85" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G85" s="16"/>
+      <c r="G85" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="H85" s="16"/>
       <c r="I85" s="20"/>
       <c r="J85" s="20"/>
@@ -21909,18 +22148,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21932,8 +22171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:AI1"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21949,7 +22188,7 @@
       <c r="C1" s="31"/>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -21961,7 +22200,7 @@
       <c r="M1" s="32"/>
       <c r="N1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
@@ -21994,13 +22233,13 @@
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>8</v>
+        <v>189</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>7</v>
+        <v>190</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
@@ -22033,25 +22272,25 @@
     </row>
     <row r="3" spans="1:35" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>187</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="5"/>
@@ -26274,18 +26513,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26297,8 +26536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26314,7 +26553,7 @@
       <c r="C1" s="31"/>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -26326,7 +26565,7 @@
       <c r="M1" s="32"/>
       <c r="N1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
@@ -26359,7 +26598,7 @@
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
@@ -26394,19 +26633,19 @@
     </row>
     <row r="3" spans="1:35" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>187</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -30303,18 +30542,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30326,11 +30565,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
@@ -30340,7 +30583,7 @@
       <c r="C1" s="31"/>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -30352,7 +30595,7 @@
       <c r="M1" s="32"/>
       <c r="N1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
@@ -30385,7 +30628,7 @@
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
@@ -30420,19 +30663,19 @@
     </row>
     <row r="3" spans="1:35" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>187</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -30761,7 +31004,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
@@ -30808,7 +31051,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
@@ -34329,18 +34572,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34352,8 +34595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34366,7 +34609,7 @@
       <c r="C1" s="31"/>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -34378,7 +34621,7 @@
       <c r="M1" s="32"/>
       <c r="N1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
@@ -34411,10 +34654,10 @@
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>5</v>
+        <v>184</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
@@ -34448,22 +34691,22 @@
     </row>
     <row r="3" spans="1:35" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>187</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>15</v>
+        <v>197</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -35734,10 +35977,10 @@
         <v>71</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -38523,18 +38766,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38546,8 +38789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38564,7 +38807,7 @@
       <c r="C1" s="31"/>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -38576,7 +38819,7 @@
       <c r="M1" s="32"/>
       <c r="N1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
@@ -38609,22 +38852,22 @@
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>5</v>
+        <v>184</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>7</v>
+        <v>190</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
@@ -38654,34 +38897,34 @@
     </row>
     <row r="3" spans="1:35" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="H3" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -43393,18 +43636,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43416,8 +43659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43433,7 +43676,7 @@
       <c r="C1" s="31"/>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -43445,7 +43688,7 @@
       <c r="M1" s="32"/>
       <c r="N1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
@@ -43478,7 +43721,7 @@
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
@@ -43513,19 +43756,19 @@
     </row>
     <row r="3" spans="1:35" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>187</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -47422,18 +47665,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47445,11 +47688,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:AI1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
@@ -47459,7 +47706,7 @@
       <c r="C1" s="31"/>
       <c r="D1" s="29"/>
       <c r="E1" s="28" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
@@ -47471,7 +47718,7 @@
       <c r="M1" s="32"/>
       <c r="N1" s="29"/>
       <c r="O1" s="28" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
@@ -47504,7 +47751,7 @@
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
@@ -47539,19 +47786,19 @@
     </row>
     <row r="3" spans="1:35" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>187</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -47927,7 +48174,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
@@ -48773,7 +49020,7 @@
         <v>71</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
@@ -48820,7 +49067,7 @@
         <v>73</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
@@ -51448,18 +51695,18 @@
     <mergeCell ref="E1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AI3 I4:AI73">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AI85">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>